<commit_message>
added nov and dec 2021
</commit_message>
<xml_diff>
--- a/GW_seaweed_seasonality_transect_data.xlsx
+++ b/GW_seaweed_seasonality_transect_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24722"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,10 +15,19 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -33,10 +42,7 @@
     <t>transect_id</t>
   </si>
   <si>
-    <t>fucus_distichus</t>
-  </si>
-  <si>
-    <t>ulva_fenestrata</t>
+    <t>distance_along_transect_m</t>
   </si>
   <si>
     <t>dominant_seaweed</t>
@@ -45,29 +51,32 @@
     <t>fucus_distichus_percent-cover</t>
   </si>
   <si>
+    <t>mastocarpus_sp_percent-cover</t>
+  </si>
+  <si>
     <t>ulva_fenestrata_percent-cover</t>
+  </si>
+  <si>
+    <t>polysiphonia_sp</t>
+  </si>
+  <si>
+    <t>fucus_distichus</t>
+  </si>
+  <si>
+    <t>no_seaweed</t>
   </si>
   <si>
     <t>mastocarpus_sp</t>
   </si>
   <si>
-    <t>mastocarpus_sp_percent-cover</t>
-  </si>
-  <si>
-    <t>no_seaweed</t>
-  </si>
-  <si>
-    <t>polysiphonia_sp</t>
-  </si>
-  <si>
-    <t>distance_along_transect_m</t>
+    <t>ulva_fenestrata</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -395,16 +404,16 @@
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -412,25 +421,25 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="F1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>44444</v>
       </c>
@@ -441,7 +450,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -450,7 +459,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>44444</v>
       </c>
@@ -464,7 +473,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>44444</v>
       </c>
@@ -478,7 +487,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>44444</v>
       </c>
@@ -489,13 +498,13 @@
         <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E5">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>44444</v>
       </c>
@@ -509,7 +518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>44444</v>
       </c>
@@ -523,7 +532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>44444</v>
       </c>
@@ -534,7 +543,7 @@
         <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E8">
         <v>2</v>
@@ -546,7 +555,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>44444</v>
       </c>
@@ -557,7 +566,7 @@
         <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>40</v>
@@ -566,7 +575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>44444</v>
       </c>
@@ -577,13 +586,13 @@
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>44444</v>
       </c>
@@ -594,13 +603,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>44444</v>
       </c>
@@ -611,7 +620,7 @@
         <v>15</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E12">
         <v>2</v>
@@ -620,7 +629,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8">
       <c r="A13" s="1">
         <v>44444</v>
       </c>
@@ -631,7 +640,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -640,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8">
       <c r="A14" s="1">
         <v>44444</v>
       </c>
@@ -651,7 +660,7 @@
         <v>25</v>
       </c>
       <c r="D14" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E14">
         <v>10</v>
@@ -660,7 +669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8">
       <c r="A15" s="1">
         <v>44444</v>
       </c>
@@ -671,7 +680,7 @@
         <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -680,7 +689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8">
       <c r="A16" s="1">
         <v>44444</v>
       </c>
@@ -691,7 +700,7 @@
         <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E16">
         <v>70</v>
@@ -700,7 +709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>44444</v>
       </c>
@@ -711,13 +720,13 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>44444</v>
       </c>
@@ -728,7 +737,7 @@
         <v>10</v>
       </c>
       <c r="D18" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E18">
         <v>2</v>
@@ -737,7 +746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>44444</v>
       </c>
@@ -748,13 +757,13 @@
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G19">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>44444</v>
       </c>
@@ -765,7 +774,7 @@
         <v>20</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E20">
         <v>2</v>
@@ -774,7 +783,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>44444</v>
       </c>
@@ -785,13 +794,13 @@
         <v>25</v>
       </c>
       <c r="D21" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G21">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>44444</v>
       </c>
@@ -802,13 +811,13 @@
         <v>30</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G22">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>44444</v>
       </c>
@@ -822,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>44444</v>
       </c>
@@ -833,13 +842,13 @@
         <v>40</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>44444</v>
       </c>
@@ -850,13 +859,13 @@
         <v>45</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G25">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>44444</v>
       </c>
@@ -867,13 +876,13 @@
         <v>50</v>
       </c>
       <c r="D26" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G26">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>44444</v>
       </c>
@@ -884,13 +893,13 @@
         <v>55</v>
       </c>
       <c r="D27" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G27">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>44444</v>
       </c>
@@ -901,13 +910,13 @@
         <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G28">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>44444</v>
       </c>
@@ -918,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E29">
         <v>70</v>
@@ -927,7 +936,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>44444</v>
       </c>
@@ -938,13 +947,13 @@
         <v>5</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F30">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>44444</v>
       </c>
@@ -958,7 +967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>44444</v>
       </c>
@@ -969,7 +978,7 @@
         <v>15</v>
       </c>
       <c r="D32" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -978,7 +987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>44444</v>
       </c>
@@ -989,7 +998,7 @@
         <v>20</v>
       </c>
       <c r="D33" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F33">
         <v>1</v>
@@ -998,7 +1007,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>44444</v>
       </c>
@@ -1009,7 +1018,7 @@
         <v>25</v>
       </c>
       <c r="D34" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E34">
         <v>1</v>
@@ -1018,7 +1027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>44444</v>
       </c>
@@ -1029,7 +1038,7 @@
         <v>30</v>
       </c>
       <c r="D35" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1038,7 +1047,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>44444</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E36">
         <v>20</v>
@@ -1058,7 +1067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>44444</v>
       </c>
@@ -1069,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="D37" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E37">
         <v>25</v>
@@ -1078,7 +1087,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>44444</v>
       </c>
@@ -1089,7 +1098,7 @@
         <v>10</v>
       </c>
       <c r="D38" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E38">
         <v>5</v>
@@ -1098,7 +1107,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>44444</v>
       </c>
@@ -1109,7 +1118,7 @@
         <v>15</v>
       </c>
       <c r="D39" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E39">
         <v>2</v>
@@ -1118,7 +1127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>44444</v>
       </c>
@@ -1129,7 +1138,7 @@
         <v>20</v>
       </c>
       <c r="D40" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1138,7 +1147,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>44444</v>
       </c>
@@ -1149,13 +1158,13 @@
         <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G41">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>44444</v>
       </c>
@@ -1166,13 +1175,13 @@
         <v>30</v>
       </c>
       <c r="D42" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="G42">
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>44473</v>
       </c>
@@ -1183,7 +1192,7 @@
         <v>0</v>
       </c>
       <c r="D43" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E43">
         <v>30</v>
@@ -1192,7 +1201,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>44473</v>
       </c>
@@ -1203,7 +1212,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E44">
         <v>5</v>
@@ -1212,7 +1221,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>44473</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>44473</v>
       </c>
@@ -1237,7 +1246,7 @@
         <v>15</v>
       </c>
       <c r="D46" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E46">
         <v>10</v>
@@ -1246,7 +1255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>44473</v>
       </c>
@@ -1257,13 +1266,13 @@
         <v>20</v>
       </c>
       <c r="D47" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E47">
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>44473</v>
       </c>
@@ -1277,7 +1286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>44473</v>
       </c>
@@ -1288,7 +1297,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E49">
         <v>40</v>
@@ -1297,7 +1306,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>44473</v>
       </c>
@@ -1308,13 +1317,13 @@
         <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F50">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>44473</v>
       </c>
@@ -1325,7 +1334,7 @@
         <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E51">
         <v>20</v>
@@ -1334,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>44473</v>
       </c>
@@ -1345,7 +1354,7 @@
         <v>15</v>
       </c>
       <c r="D52" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E52">
         <v>10</v>
@@ -1354,7 +1363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>44473</v>
       </c>
@@ -1365,13 +1374,13 @@
         <v>20</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F53">
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>44473</v>
       </c>
@@ -1382,7 +1391,7 @@
         <v>25</v>
       </c>
       <c r="D54" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E54">
         <v>5</v>
@@ -1391,7 +1400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>44473</v>
       </c>
@@ -1402,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E55">
         <v>40</v>
@@ -1411,7 +1420,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
         <v>44473</v>
       </c>
@@ -1425,7 +1434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
         <v>44473</v>
       </c>
@@ -1436,7 +1445,7 @@
         <v>10</v>
       </c>
       <c r="D57" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E57">
         <v>1</v>
@@ -1445,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
         <v>44473</v>
       </c>
@@ -1456,7 +1465,7 @@
         <v>15</v>
       </c>
       <c r="D58" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -1465,7 +1474,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
         <v>44473</v>
       </c>
@@ -1476,7 +1485,7 @@
         <v>20</v>
       </c>
       <c r="D59" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E59">
         <v>5</v>
@@ -1485,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>44473</v>
       </c>
@@ -1496,7 +1505,7 @@
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E60">
         <v>70</v>
@@ -1505,7 +1514,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>44473</v>
       </c>
@@ -1516,7 +1525,7 @@
         <v>5</v>
       </c>
       <c r="D61" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E61">
         <v>1</v>
@@ -1525,7 +1534,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
         <v>44473</v>
       </c>
@@ -1536,13 +1545,13 @@
         <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E62">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>44473</v>
       </c>
@@ -1556,7 +1565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>44473</v>
       </c>
@@ -1567,7 +1576,7 @@
         <v>20</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E64">
         <v>10</v>
@@ -1579,7 +1588,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65" s="1">
         <v>44473</v>
       </c>
@@ -1590,7 +1599,7 @@
         <v>0</v>
       </c>
       <c r="D65" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E65">
         <v>40</v>
@@ -1602,7 +1611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66" s="1">
         <v>44473</v>
       </c>
@@ -1613,7 +1622,7 @@
         <v>5</v>
       </c>
       <c r="D66" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E66">
         <v>30</v>
@@ -1622,7 +1631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67" s="1">
         <v>44473</v>
       </c>
@@ -1633,7 +1642,7 @@
         <v>10</v>
       </c>
       <c r="D67" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E67">
         <v>10</v>
@@ -1642,7 +1651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8">
       <c r="A68" s="1">
         <v>44473</v>
       </c>
@@ -1653,7 +1662,7 @@
         <v>15</v>
       </c>
       <c r="D68" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E68">
         <v>5</v>

</xml_diff>

<commit_message>
repro data for app
</commit_message>
<xml_diff>
--- a/GW_seaweed_seasonality_transect_data.xlsx
+++ b/GW_seaweed_seasonality_transect_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26704"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3087" documentId="8_{66D09B87-BA6E-4AE3-AABA-E18550A91A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75DBF0F4-140E-4A23-B8FB-EBFA68E550EE}"/>
+  <xr:revisionPtr revIDLastSave="3441" documentId="8_{66D09B87-BA6E-4AE3-AABA-E18550A91A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D731B6D7-9427-4C8F-B107-70F18950A033}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="113">
   <si>
     <t>year</t>
   </si>
@@ -369,6 +369,9 @@
   </si>
   <si>
     <t>saccharina_sp</t>
+  </si>
+  <si>
+    <t>prionitis_sternbergii</t>
   </si>
 </sst>
 </file>
@@ -1231,24 +1234,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BT919"/>
+  <dimension ref="A1:BT966"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AX1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="E865" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AN881" sqref="AN881"/>
+      <pane ySplit="1" topLeftCell="A920" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AM922" sqref="AM922"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" customWidth="1"/>
-    <col min="11" max="13" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="4.7109375" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" customWidth="1"/>
+    <col min="10" max="10" width="4.5703125" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" customWidth="1"/>
+    <col min="12" max="12" width="5.28515625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="15.5703125" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="15.28515625" hidden="1" customWidth="1"/>
     <col min="17" max="17" width="13.28515625" hidden="1" customWidth="1"/>
     <col min="18" max="20" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="21" max="24" width="9.140625" customWidth="1"/>
+    <col min="21" max="21" width="4.5703125" customWidth="1"/>
+    <col min="22" max="22" width="5.7109375" customWidth="1"/>
+    <col min="23" max="23" width="5.28515625" customWidth="1"/>
+    <col min="24" max="24" width="4" customWidth="1"/>
     <col min="25" max="26" width="0" hidden="1" customWidth="1"/>
     <col min="27" max="27" width="7.7109375" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="10.42578125" hidden="1" customWidth="1"/>
@@ -1257,9 +1272,42 @@
     <col min="31" max="31" width="11.5703125" hidden="1" customWidth="1"/>
     <col min="32" max="32" width="13.7109375" hidden="1" customWidth="1"/>
     <col min="33" max="34" width="10.140625" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="14.42578125" customWidth="1"/>
+    <col min="35" max="35" width="13.5703125" customWidth="1"/>
     <col min="36" max="36" width="14.28515625" customWidth="1"/>
-    <col min="37" max="37" width="11.28515625" customWidth="1"/>
+    <col min="37" max="37" width="11.28515625" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="6.140625" customWidth="1"/>
+    <col min="39" max="39" width="5.85546875" customWidth="1"/>
+    <col min="40" max="40" width="5.140625" customWidth="1"/>
+    <col min="41" max="41" width="5.28515625" customWidth="1"/>
+    <col min="42" max="42" width="5.42578125" customWidth="1"/>
+    <col min="43" max="43" width="6.42578125" customWidth="1"/>
+    <col min="44" max="44" width="4.28515625" customWidth="1"/>
+    <col min="47" max="47" width="6.85546875" customWidth="1"/>
+    <col min="48" max="48" width="5.5703125" customWidth="1"/>
+    <col min="49" max="49" width="7.85546875" customWidth="1"/>
+    <col min="50" max="50" width="6.85546875" customWidth="1"/>
+    <col min="51" max="51" width="7.42578125" customWidth="1"/>
+    <col min="52" max="52" width="7.28515625" customWidth="1"/>
+    <col min="53" max="53" width="6.140625" customWidth="1"/>
+    <col min="54" max="54" width="7.5703125" customWidth="1"/>
+    <col min="55" max="55" width="7" customWidth="1"/>
+    <col min="56" max="56" width="6.42578125" customWidth="1"/>
+    <col min="57" max="57" width="6" customWidth="1"/>
+    <col min="58" max="58" width="6.28515625" customWidth="1"/>
+    <col min="59" max="59" width="6.140625" customWidth="1"/>
+    <col min="60" max="60" width="6.7109375" customWidth="1"/>
+    <col min="61" max="61" width="6.28515625" customWidth="1"/>
+    <col min="62" max="62" width="5.5703125" customWidth="1"/>
+    <col min="63" max="63" width="6.28515625" customWidth="1"/>
+    <col min="64" max="64" width="6.7109375" customWidth="1"/>
+    <col min="65" max="65" width="5.85546875" customWidth="1"/>
+    <col min="66" max="66" width="7" customWidth="1"/>
+    <col min="67" max="67" width="6.5703125" customWidth="1"/>
+    <col min="68" max="68" width="6.140625" customWidth="1"/>
+    <col min="69" max="69" width="4.42578125" customWidth="1"/>
+    <col min="70" max="70" width="4.140625" customWidth="1"/>
+    <col min="71" max="71" width="5.85546875" customWidth="1"/>
+    <col min="72" max="72" width="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:72">
@@ -36295,7 +36343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="881" spans="1:7">
+    <row r="881" spans="1:50">
       <c r="A881">
         <v>2023</v>
       </c>
@@ -36317,8 +36365,29 @@
       <c r="G881">
         <v>30</v>
       </c>
-    </row>
-    <row r="882" spans="1:7">
+      <c r="H881" t="s">
+        <v>110</v>
+      </c>
+      <c r="I881">
+        <v>3</v>
+      </c>
+      <c r="O881">
+        <v>1</v>
+      </c>
+      <c r="X881">
+        <v>50</v>
+      </c>
+      <c r="AL881">
+        <v>5</v>
+      </c>
+      <c r="AV881">
+        <v>1</v>
+      </c>
+      <c r="AW881">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="882" spans="1:50">
       <c r="A882">
         <v>2023</v>
       </c>
@@ -36340,8 +36409,23 @@
       <c r="G882">
         <v>35</v>
       </c>
-    </row>
-    <row r="883" spans="1:7">
+      <c r="H882" t="s">
+        <v>110</v>
+      </c>
+      <c r="I882">
+        <v>10</v>
+      </c>
+      <c r="X882">
+        <v>70</v>
+      </c>
+      <c r="AL882">
+        <v>15</v>
+      </c>
+      <c r="AM882">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="883" spans="1:50">
       <c r="A883">
         <v>2023</v>
       </c>
@@ -36363,8 +36447,26 @@
       <c r="G883">
         <v>40</v>
       </c>
-    </row>
-    <row r="884" spans="1:7">
+      <c r="I883">
+        <v>5</v>
+      </c>
+      <c r="J883">
+        <v>2</v>
+      </c>
+      <c r="X883">
+        <v>20</v>
+      </c>
+      <c r="AL883">
+        <v>20</v>
+      </c>
+      <c r="AQ883">
+        <v>2</v>
+      </c>
+      <c r="AX883">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="884" spans="1:50">
       <c r="A884">
         <v>2023</v>
       </c>
@@ -36386,8 +36488,23 @@
       <c r="G884">
         <v>0</v>
       </c>
-    </row>
-    <row r="885" spans="1:7">
+      <c r="I884">
+        <v>5</v>
+      </c>
+      <c r="X884">
+        <v>5</v>
+      </c>
+      <c r="AL884">
+        <v>3</v>
+      </c>
+      <c r="AM884">
+        <v>2</v>
+      </c>
+      <c r="AN884">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="885" spans="1:50">
       <c r="A885">
         <v>2023</v>
       </c>
@@ -36409,8 +36526,23 @@
       <c r="G885">
         <v>5</v>
       </c>
-    </row>
-    <row r="886" spans="1:7">
+      <c r="H885" t="s">
+        <v>110</v>
+      </c>
+      <c r="I885">
+        <v>2</v>
+      </c>
+      <c r="X885">
+        <v>70</v>
+      </c>
+      <c r="AL885">
+        <v>1</v>
+      </c>
+      <c r="AN885">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="886" spans="1:50">
       <c r="A886">
         <v>2023</v>
       </c>
@@ -36432,8 +36564,23 @@
       <c r="G886">
         <v>10</v>
       </c>
-    </row>
-    <row r="887" spans="1:7">
+      <c r="H886" t="s">
+        <v>110</v>
+      </c>
+      <c r="I886">
+        <v>2</v>
+      </c>
+      <c r="X886">
+        <v>80</v>
+      </c>
+      <c r="AL886">
+        <v>2</v>
+      </c>
+      <c r="AN886">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="887" spans="1:50">
       <c r="A887">
         <v>2023</v>
       </c>
@@ -36455,8 +36602,23 @@
       <c r="G887">
         <v>15</v>
       </c>
-    </row>
-    <row r="888" spans="1:7">
+      <c r="H887" t="s">
+        <v>110</v>
+      </c>
+      <c r="I887">
+        <v>3</v>
+      </c>
+      <c r="X887">
+        <v>70</v>
+      </c>
+      <c r="AL887">
+        <v>1</v>
+      </c>
+      <c r="AN887">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="888" spans="1:50">
       <c r="A888">
         <v>2023</v>
       </c>
@@ -36478,8 +36640,17 @@
       <c r="G888">
         <v>20</v>
       </c>
-    </row>
-    <row r="889" spans="1:7">
+      <c r="H888" t="s">
+        <v>110</v>
+      </c>
+      <c r="X888">
+        <v>70</v>
+      </c>
+      <c r="AN888">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="889" spans="1:50">
       <c r="A889">
         <v>2023</v>
       </c>
@@ -36501,8 +36672,20 @@
       <c r="G889">
         <v>25</v>
       </c>
-    </row>
-    <row r="890" spans="1:7">
+      <c r="H889" t="s">
+        <v>110</v>
+      </c>
+      <c r="I889">
+        <v>1</v>
+      </c>
+      <c r="X889">
+        <v>40</v>
+      </c>
+      <c r="AL889">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="890" spans="1:50">
       <c r="A890">
         <v>2023</v>
       </c>
@@ -36524,8 +36707,26 @@
       <c r="G890">
         <v>30</v>
       </c>
-    </row>
-    <row r="891" spans="1:7">
+      <c r="H890" t="s">
+        <v>110</v>
+      </c>
+      <c r="I890">
+        <v>1</v>
+      </c>
+      <c r="X890">
+        <v>30</v>
+      </c>
+      <c r="AL890">
+        <v>1</v>
+      </c>
+      <c r="AN890">
+        <v>1</v>
+      </c>
+      <c r="AO890">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="891" spans="1:50">
       <c r="A891">
         <v>2023</v>
       </c>
@@ -36547,8 +36748,17 @@
       <c r="G891">
         <v>35</v>
       </c>
-    </row>
-    <row r="892" spans="1:7">
+      <c r="H891" t="s">
+        <v>110</v>
+      </c>
+      <c r="X891">
+        <v>10</v>
+      </c>
+      <c r="AL891">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="892" spans="1:50">
       <c r="A892">
         <v>2023</v>
       </c>
@@ -36570,8 +36780,23 @@
       <c r="G892">
         <v>40</v>
       </c>
-    </row>
-    <row r="893" spans="1:7">
+      <c r="H892" t="s">
+        <v>110</v>
+      </c>
+      <c r="J892">
+        <v>2</v>
+      </c>
+      <c r="X892">
+        <v>10</v>
+      </c>
+      <c r="AL892">
+        <v>1</v>
+      </c>
+      <c r="AM892">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="893" spans="1:50">
       <c r="A893">
         <v>2023</v>
       </c>
@@ -36593,8 +36818,20 @@
       <c r="G893">
         <v>45</v>
       </c>
-    </row>
-    <row r="894" spans="1:7">
+      <c r="H893" t="s">
+        <v>110</v>
+      </c>
+      <c r="J893">
+        <v>1</v>
+      </c>
+      <c r="X893">
+        <v>40</v>
+      </c>
+      <c r="AL893">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="894" spans="1:50">
       <c r="A894">
         <v>2023</v>
       </c>
@@ -36616,8 +36853,23 @@
       <c r="G894">
         <v>50</v>
       </c>
-    </row>
-    <row r="895" spans="1:7">
+      <c r="H894" t="s">
+        <v>110</v>
+      </c>
+      <c r="I894">
+        <v>5</v>
+      </c>
+      <c r="X894">
+        <v>40</v>
+      </c>
+      <c r="AL894">
+        <v>5</v>
+      </c>
+      <c r="AM894">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="895" spans="1:50">
       <c r="A895">
         <v>2023</v>
       </c>
@@ -36639,8 +36891,26 @@
       <c r="G895">
         <v>55</v>
       </c>
-    </row>
-    <row r="896" spans="1:7">
+      <c r="H895" t="s">
+        <v>110</v>
+      </c>
+      <c r="I895">
+        <v>1</v>
+      </c>
+      <c r="J895">
+        <v>2</v>
+      </c>
+      <c r="X895">
+        <v>60</v>
+      </c>
+      <c r="AL895">
+        <v>5</v>
+      </c>
+      <c r="AV895">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="896" spans="1:50">
       <c r="A896">
         <v>2023</v>
       </c>
@@ -36662,8 +36932,29 @@
       <c r="G896">
         <v>60</v>
       </c>
-    </row>
-    <row r="897" spans="1:7">
+      <c r="H896" t="s">
+        <v>110</v>
+      </c>
+      <c r="I896">
+        <v>1</v>
+      </c>
+      <c r="J896">
+        <v>5</v>
+      </c>
+      <c r="X896">
+        <v>80</v>
+      </c>
+      <c r="AL896">
+        <v>3</v>
+      </c>
+      <c r="AV896">
+        <v>1</v>
+      </c>
+      <c r="AX896">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="897" spans="1:69">
       <c r="A897">
         <v>2023</v>
       </c>
@@ -36685,8 +36976,17 @@
       <c r="G897">
         <v>65</v>
       </c>
-    </row>
-    <row r="898" spans="1:7">
+      <c r="H897" t="s">
+        <v>110</v>
+      </c>
+      <c r="J897">
+        <v>5</v>
+      </c>
+      <c r="X897">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="898" spans="1:69">
       <c r="A898">
         <v>2023</v>
       </c>
@@ -36708,8 +37008,20 @@
       <c r="G898">
         <v>70</v>
       </c>
-    </row>
-    <row r="899" spans="1:7">
+      <c r="H898" t="s">
+        <v>110</v>
+      </c>
+      <c r="J898">
+        <v>10</v>
+      </c>
+      <c r="X898">
+        <v>90</v>
+      </c>
+      <c r="BP898">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="899" spans="1:69">
       <c r="A899">
         <v>2023</v>
       </c>
@@ -36731,8 +37043,26 @@
       <c r="G899">
         <v>75</v>
       </c>
-    </row>
-    <row r="900" spans="1:7">
+      <c r="H899" t="s">
+        <v>93</v>
+      </c>
+      <c r="J899">
+        <v>60</v>
+      </c>
+      <c r="AP899">
+        <v>5</v>
+      </c>
+      <c r="AQ899">
+        <v>10</v>
+      </c>
+      <c r="AS899">
+        <v>1</v>
+      </c>
+      <c r="AX899">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="900" spans="1:69">
       <c r="A900">
         <v>2023</v>
       </c>
@@ -36754,8 +37084,50 @@
       <c r="G900">
         <v>80</v>
       </c>
-    </row>
-    <row r="901" spans="1:7">
+      <c r="H900" t="s">
+        <v>93</v>
+      </c>
+      <c r="I900">
+        <v>2</v>
+      </c>
+      <c r="J900">
+        <v>30</v>
+      </c>
+      <c r="K900">
+        <v>1</v>
+      </c>
+      <c r="L900">
+        <v>3</v>
+      </c>
+      <c r="X900">
+        <v>2</v>
+      </c>
+      <c r="AL900">
+        <v>2</v>
+      </c>
+      <c r="AP900">
+        <v>1</v>
+      </c>
+      <c r="AQ900">
+        <v>3</v>
+      </c>
+      <c r="AS900">
+        <v>1</v>
+      </c>
+      <c r="AV900">
+        <v>5</v>
+      </c>
+      <c r="AX900">
+        <v>2</v>
+      </c>
+      <c r="BC900">
+        <v>5</v>
+      </c>
+      <c r="BO900">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="901" spans="1:69">
       <c r="A901">
         <v>2023</v>
       </c>
@@ -36777,8 +37149,47 @@
       <c r="G901">
         <v>85</v>
       </c>
-    </row>
-    <row r="902" spans="1:7">
+      <c r="H901" t="s">
+        <v>112</v>
+      </c>
+      <c r="J901">
+        <v>3</v>
+      </c>
+      <c r="K901">
+        <v>5</v>
+      </c>
+      <c r="L901">
+        <v>1</v>
+      </c>
+      <c r="X901">
+        <v>15</v>
+      </c>
+      <c r="AL901">
+        <v>5</v>
+      </c>
+      <c r="AM901">
+        <v>3</v>
+      </c>
+      <c r="AQ901">
+        <v>2</v>
+      </c>
+      <c r="AR901">
+        <v>15</v>
+      </c>
+      <c r="AS901">
+        <v>20</v>
+      </c>
+      <c r="BC901">
+        <v>2</v>
+      </c>
+      <c r="BL901">
+        <v>1</v>
+      </c>
+      <c r="BO901">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="902" spans="1:69">
       <c r="A902">
         <v>2023</v>
       </c>
@@ -36800,8 +37211,50 @@
       <c r="G902">
         <v>90</v>
       </c>
-    </row>
-    <row r="903" spans="1:7">
+      <c r="H902" t="s">
+        <v>96</v>
+      </c>
+      <c r="I902">
+        <v>5</v>
+      </c>
+      <c r="J902">
+        <v>20</v>
+      </c>
+      <c r="K902">
+        <v>100</v>
+      </c>
+      <c r="L902">
+        <v>15</v>
+      </c>
+      <c r="X902">
+        <v>15</v>
+      </c>
+      <c r="AL902">
+        <v>10</v>
+      </c>
+      <c r="AM902">
+        <v>10</v>
+      </c>
+      <c r="AP902">
+        <v>1</v>
+      </c>
+      <c r="AQ902">
+        <v>5</v>
+      </c>
+      <c r="AV902">
+        <v>2</v>
+      </c>
+      <c r="AX902">
+        <v>1</v>
+      </c>
+      <c r="BC902">
+        <v>1</v>
+      </c>
+      <c r="BO902">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="903" spans="1:69">
       <c r="A903">
         <v>2023</v>
       </c>
@@ -36823,8 +37276,23 @@
       <c r="G903">
         <v>0</v>
       </c>
-    </row>
-    <row r="904" spans="1:7">
+      <c r="I903">
+        <v>7</v>
+      </c>
+      <c r="X903">
+        <v>10</v>
+      </c>
+      <c r="AL903">
+        <v>5</v>
+      </c>
+      <c r="AV903">
+        <v>1</v>
+      </c>
+      <c r="AW903">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="904" spans="1:69">
       <c r="A904">
         <v>2023</v>
       </c>
@@ -36846,8 +37314,17 @@
       <c r="G904">
         <v>5</v>
       </c>
-    </row>
-    <row r="905" spans="1:7">
+      <c r="H904" t="s">
+        <v>110</v>
+      </c>
+      <c r="X904">
+        <v>20</v>
+      </c>
+      <c r="AL904">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="905" spans="1:69">
       <c r="A905">
         <v>2023</v>
       </c>
@@ -36869,8 +37346,23 @@
       <c r="G905">
         <v>10</v>
       </c>
-    </row>
-    <row r="906" spans="1:7">
+      <c r="H905" t="s">
+        <v>110</v>
+      </c>
+      <c r="X905">
+        <v>85</v>
+      </c>
+      <c r="AL905">
+        <v>1</v>
+      </c>
+      <c r="AN905">
+        <v>2</v>
+      </c>
+      <c r="AV905">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="906" spans="1:69">
       <c r="A906">
         <v>2023</v>
       </c>
@@ -36892,8 +37384,26 @@
       <c r="G906">
         <v>15</v>
       </c>
-    </row>
-    <row r="907" spans="1:7">
+      <c r="H906" t="s">
+        <v>110</v>
+      </c>
+      <c r="I906">
+        <v>1</v>
+      </c>
+      <c r="X906">
+        <v>75</v>
+      </c>
+      <c r="AL906">
+        <v>2</v>
+      </c>
+      <c r="AN906">
+        <v>1</v>
+      </c>
+      <c r="AV906">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="907" spans="1:69">
       <c r="A907">
         <v>2023</v>
       </c>
@@ -36915,8 +37425,23 @@
       <c r="G907">
         <v>20</v>
       </c>
-    </row>
-    <row r="908" spans="1:7">
+      <c r="H907" t="s">
+        <v>110</v>
+      </c>
+      <c r="I907">
+        <v>3</v>
+      </c>
+      <c r="X907">
+        <v>60</v>
+      </c>
+      <c r="AL907">
+        <v>5</v>
+      </c>
+      <c r="AN907">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="908" spans="1:69">
       <c r="A908">
         <v>2023</v>
       </c>
@@ -36938,8 +37463,20 @@
       <c r="G908">
         <v>25</v>
       </c>
-    </row>
-    <row r="909" spans="1:7">
+      <c r="H908" t="s">
+        <v>110</v>
+      </c>
+      <c r="X908">
+        <v>80</v>
+      </c>
+      <c r="AI908">
+        <v>1</v>
+      </c>
+      <c r="AL908">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="909" spans="1:69">
       <c r="A909">
         <v>2023</v>
       </c>
@@ -36961,8 +37498,26 @@
       <c r="G909">
         <v>30</v>
       </c>
-    </row>
-    <row r="910" spans="1:7">
+      <c r="H909" t="s">
+        <v>110</v>
+      </c>
+      <c r="I909">
+        <v>1</v>
+      </c>
+      <c r="X909">
+        <v>70</v>
+      </c>
+      <c r="AL909">
+        <v>2</v>
+      </c>
+      <c r="AV909">
+        <v>1</v>
+      </c>
+      <c r="AX909">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="910" spans="1:69">
       <c r="A910">
         <v>2023</v>
       </c>
@@ -36984,8 +37539,23 @@
       <c r="G910">
         <v>35</v>
       </c>
-    </row>
-    <row r="911" spans="1:7">
+      <c r="H910" t="s">
+        <v>110</v>
+      </c>
+      <c r="X910">
+        <v>35</v>
+      </c>
+      <c r="AL910">
+        <v>5</v>
+      </c>
+      <c r="AM910">
+        <v>1</v>
+      </c>
+      <c r="AX910">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="911" spans="1:69">
       <c r="A911">
         <v>2023</v>
       </c>
@@ -37007,8 +37577,26 @@
       <c r="G911">
         <v>40</v>
       </c>
-    </row>
-    <row r="912" spans="1:7">
+      <c r="H911" t="s">
+        <v>110</v>
+      </c>
+      <c r="X911">
+        <v>60</v>
+      </c>
+      <c r="AL911">
+        <v>3</v>
+      </c>
+      <c r="AM911">
+        <v>1</v>
+      </c>
+      <c r="AV911">
+        <v>1</v>
+      </c>
+      <c r="BQ911">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="912" spans="1:69">
       <c r="A912">
         <v>2023</v>
       </c>
@@ -37030,8 +37618,29 @@
       <c r="G912">
         <v>45</v>
       </c>
-    </row>
-    <row r="913" spans="1:7">
+      <c r="H912" t="s">
+        <v>110</v>
+      </c>
+      <c r="J912">
+        <v>2</v>
+      </c>
+      <c r="X912">
+        <v>70</v>
+      </c>
+      <c r="AL912">
+        <v>3</v>
+      </c>
+      <c r="AM912">
+        <v>1</v>
+      </c>
+      <c r="AV912">
+        <v>1</v>
+      </c>
+      <c r="AX912">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="913" spans="1:67">
       <c r="A913">
         <v>2023</v>
       </c>
@@ -37053,8 +37662,26 @@
       <c r="G913">
         <v>50</v>
       </c>
-    </row>
-    <row r="914" spans="1:7">
+      <c r="H913" t="s">
+        <v>110</v>
+      </c>
+      <c r="X913">
+        <v>75</v>
+      </c>
+      <c r="AL913">
+        <v>1</v>
+      </c>
+      <c r="AN913">
+        <v>3</v>
+      </c>
+      <c r="AV913">
+        <v>1</v>
+      </c>
+      <c r="AX913">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="914" spans="1:67">
       <c r="A914">
         <v>2023</v>
       </c>
@@ -37076,8 +37703,26 @@
       <c r="G914">
         <v>55</v>
       </c>
-    </row>
-    <row r="915" spans="1:7">
+      <c r="H914" t="s">
+        <v>110</v>
+      </c>
+      <c r="I914">
+        <v>1</v>
+      </c>
+      <c r="J914">
+        <v>5</v>
+      </c>
+      <c r="X914">
+        <v>55</v>
+      </c>
+      <c r="AL914">
+        <v>3</v>
+      </c>
+      <c r="AX914">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="915" spans="1:67">
       <c r="A915">
         <v>2023</v>
       </c>
@@ -37099,8 +37744,29 @@
       <c r="G915">
         <v>60</v>
       </c>
-    </row>
-    <row r="916" spans="1:7">
+      <c r="H915" t="s">
+        <v>110</v>
+      </c>
+      <c r="I915">
+        <v>2</v>
+      </c>
+      <c r="J915">
+        <v>5</v>
+      </c>
+      <c r="X915">
+        <v>40</v>
+      </c>
+      <c r="AL915">
+        <v>10</v>
+      </c>
+      <c r="AV915">
+        <v>30</v>
+      </c>
+      <c r="AX915">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="916" spans="1:67">
       <c r="A916">
         <v>2023</v>
       </c>
@@ -37122,8 +37788,29 @@
       <c r="G916">
         <v>65</v>
       </c>
-    </row>
-    <row r="917" spans="1:7">
+      <c r="H916" t="s">
+        <v>110</v>
+      </c>
+      <c r="J916">
+        <v>20</v>
+      </c>
+      <c r="K916">
+        <v>5</v>
+      </c>
+      <c r="X916">
+        <v>70</v>
+      </c>
+      <c r="AL916">
+        <v>1</v>
+      </c>
+      <c r="AX916">
+        <v>2</v>
+      </c>
+      <c r="BO916">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="917" spans="1:67">
       <c r="A917">
         <v>2023</v>
       </c>
@@ -37145,8 +37832,32 @@
       <c r="G917">
         <v>70</v>
       </c>
-    </row>
-    <row r="918" spans="1:7">
+      <c r="H917" t="s">
+        <v>110</v>
+      </c>
+      <c r="J917">
+        <v>20</v>
+      </c>
+      <c r="U917">
+        <v>1</v>
+      </c>
+      <c r="X917">
+        <v>70</v>
+      </c>
+      <c r="AL917">
+        <v>1</v>
+      </c>
+      <c r="AS917">
+        <v>1</v>
+      </c>
+      <c r="AX917">
+        <v>2</v>
+      </c>
+      <c r="BO917">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="918" spans="1:67">
       <c r="A918">
         <v>2023</v>
       </c>
@@ -37168,8 +37879,38 @@
       <c r="G918">
         <v>75</v>
       </c>
-    </row>
-    <row r="919" spans="1:7">
+      <c r="H918" t="s">
+        <v>93</v>
+      </c>
+      <c r="J918">
+        <v>30</v>
+      </c>
+      <c r="K918">
+        <v>20</v>
+      </c>
+      <c r="X918">
+        <v>20</v>
+      </c>
+      <c r="AL918">
+        <v>5</v>
+      </c>
+      <c r="AQ918">
+        <v>5</v>
+      </c>
+      <c r="AR918">
+        <v>5</v>
+      </c>
+      <c r="AV918">
+        <v>1</v>
+      </c>
+      <c r="AX918">
+        <v>10</v>
+      </c>
+      <c r="BO918">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="919" spans="1:67">
       <c r="A919">
         <v>2023</v>
       </c>
@@ -37190,6 +37931,1159 @@
       </c>
       <c r="G919">
         <v>80</v>
+      </c>
+      <c r="H919" t="s">
+        <v>110</v>
+      </c>
+      <c r="J919">
+        <v>15</v>
+      </c>
+      <c r="U919">
+        <v>1</v>
+      </c>
+      <c r="X919">
+        <v>90</v>
+      </c>
+      <c r="AL919">
+        <v>2</v>
+      </c>
+      <c r="AR919">
+        <v>2</v>
+      </c>
+      <c r="AV919">
+        <v>1</v>
+      </c>
+      <c r="AX919">
+        <v>2</v>
+      </c>
+      <c r="BO919">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="920" spans="1:67">
+      <c r="A920">
+        <v>2023</v>
+      </c>
+      <c r="B920">
+        <v>7</v>
+      </c>
+      <c r="C920">
+        <v>4</v>
+      </c>
+      <c r="D920" s="3">
+        <v>0.55416666666666703</v>
+      </c>
+      <c r="E920">
+        <v>0</v>
+      </c>
+      <c r="F920">
+        <v>4</v>
+      </c>
+      <c r="G920">
+        <v>85</v>
+      </c>
+      <c r="H920" t="s">
+        <v>93</v>
+      </c>
+      <c r="J920">
+        <v>30</v>
+      </c>
+      <c r="U920">
+        <v>15</v>
+      </c>
+      <c r="X920">
+        <v>5</v>
+      </c>
+      <c r="AP920">
+        <v>2</v>
+      </c>
+      <c r="AQ920">
+        <v>2</v>
+      </c>
+      <c r="AS920">
+        <v>5</v>
+      </c>
+      <c r="AX920">
+        <v>1</v>
+      </c>
+      <c r="BC920">
+        <v>5</v>
+      </c>
+      <c r="BD920">
+        <v>10</v>
+      </c>
+      <c r="BL920">
+        <v>2</v>
+      </c>
+      <c r="BO920">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="921" spans="1:67">
+      <c r="A921">
+        <v>2023</v>
+      </c>
+      <c r="B921">
+        <v>8</v>
+      </c>
+      <c r="C921">
+        <v>1</v>
+      </c>
+      <c r="D921" s="3">
+        <v>0.51111111111111118</v>
+      </c>
+      <c r="E921">
+        <v>0.1</v>
+      </c>
+      <c r="F921">
+        <v>2</v>
+      </c>
+      <c r="G921">
+        <v>0</v>
+      </c>
+      <c r="H921" t="s">
+        <v>72</v>
+      </c>
+      <c r="I921">
+        <v>10</v>
+      </c>
+      <c r="AM921">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="922" spans="1:67">
+      <c r="A922">
+        <v>2023</v>
+      </c>
+      <c r="B922">
+        <v>8</v>
+      </c>
+      <c r="C922">
+        <v>1</v>
+      </c>
+      <c r="D922" s="3">
+        <v>0.51111111111111118</v>
+      </c>
+      <c r="E922">
+        <v>0.1</v>
+      </c>
+      <c r="F922">
+        <v>2</v>
+      </c>
+      <c r="G922">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="923" spans="1:67">
+      <c r="A923">
+        <v>2023</v>
+      </c>
+      <c r="B923">
+        <v>8</v>
+      </c>
+      <c r="C923">
+        <v>1</v>
+      </c>
+      <c r="D923" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E923">
+        <v>0.1</v>
+      </c>
+      <c r="F923">
+        <v>2</v>
+      </c>
+      <c r="G923">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="924" spans="1:67">
+      <c r="A924">
+        <v>2023</v>
+      </c>
+      <c r="B924">
+        <v>8</v>
+      </c>
+      <c r="C924">
+        <v>1</v>
+      </c>
+      <c r="D924" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E924">
+        <v>0.1</v>
+      </c>
+      <c r="F924">
+        <v>2</v>
+      </c>
+      <c r="G924">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="925" spans="1:67">
+      <c r="A925">
+        <v>2023</v>
+      </c>
+      <c r="B925">
+        <v>8</v>
+      </c>
+      <c r="C925">
+        <v>1</v>
+      </c>
+      <c r="D925" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E925">
+        <v>0.1</v>
+      </c>
+      <c r="F925">
+        <v>2</v>
+      </c>
+      <c r="G925">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="926" spans="1:67">
+      <c r="A926">
+        <v>2023</v>
+      </c>
+      <c r="B926">
+        <v>8</v>
+      </c>
+      <c r="C926">
+        <v>1</v>
+      </c>
+      <c r="D926" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E926">
+        <v>0.1</v>
+      </c>
+      <c r="F926">
+        <v>2</v>
+      </c>
+      <c r="G926">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="927" spans="1:67">
+      <c r="A927">
+        <v>2023</v>
+      </c>
+      <c r="B927">
+        <v>8</v>
+      </c>
+      <c r="C927">
+        <v>1</v>
+      </c>
+      <c r="D927" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E927">
+        <v>0.1</v>
+      </c>
+      <c r="F927">
+        <v>2</v>
+      </c>
+      <c r="G927">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="928" spans="1:67">
+      <c r="A928">
+        <v>2023</v>
+      </c>
+      <c r="B928">
+        <v>8</v>
+      </c>
+      <c r="C928">
+        <v>1</v>
+      </c>
+      <c r="D928" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E928">
+        <v>0.1</v>
+      </c>
+      <c r="F928">
+        <v>2</v>
+      </c>
+      <c r="G928">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="929" spans="1:7">
+      <c r="A929">
+        <v>2023</v>
+      </c>
+      <c r="B929">
+        <v>8</v>
+      </c>
+      <c r="C929">
+        <v>1</v>
+      </c>
+      <c r="D929" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E929">
+        <v>0.1</v>
+      </c>
+      <c r="F929">
+        <v>2</v>
+      </c>
+      <c r="G929">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="930" spans="1:7">
+      <c r="A930">
+        <v>2023</v>
+      </c>
+      <c r="B930">
+        <v>8</v>
+      </c>
+      <c r="C930">
+        <v>1</v>
+      </c>
+      <c r="D930" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E930">
+        <v>0.1</v>
+      </c>
+      <c r="F930">
+        <v>3</v>
+      </c>
+      <c r="G930">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="931" spans="1:7">
+      <c r="A931">
+        <v>2023</v>
+      </c>
+      <c r="B931">
+        <v>8</v>
+      </c>
+      <c r="C931">
+        <v>1</v>
+      </c>
+      <c r="D931" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E931">
+        <v>0.1</v>
+      </c>
+      <c r="F931">
+        <v>3</v>
+      </c>
+      <c r="G931">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="932" spans="1:7">
+      <c r="A932">
+        <v>2023</v>
+      </c>
+      <c r="B932">
+        <v>8</v>
+      </c>
+      <c r="C932">
+        <v>1</v>
+      </c>
+      <c r="D932" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E932">
+        <v>0.1</v>
+      </c>
+      <c r="F932">
+        <v>3</v>
+      </c>
+      <c r="G932">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="933" spans="1:7">
+      <c r="A933">
+        <v>2023</v>
+      </c>
+      <c r="B933">
+        <v>8</v>
+      </c>
+      <c r="C933">
+        <v>1</v>
+      </c>
+      <c r="D933" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E933">
+        <v>0.1</v>
+      </c>
+      <c r="F933">
+        <v>3</v>
+      </c>
+      <c r="G933">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="934" spans="1:7">
+      <c r="A934">
+        <v>2023</v>
+      </c>
+      <c r="B934">
+        <v>8</v>
+      </c>
+      <c r="C934">
+        <v>1</v>
+      </c>
+      <c r="D934" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E934">
+        <v>0.1</v>
+      </c>
+      <c r="F934">
+        <v>3</v>
+      </c>
+      <c r="G934">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="935" spans="1:7">
+      <c r="A935">
+        <v>2023</v>
+      </c>
+      <c r="B935">
+        <v>8</v>
+      </c>
+      <c r="C935">
+        <v>1</v>
+      </c>
+      <c r="D935" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E935">
+        <v>0.1</v>
+      </c>
+      <c r="F935">
+        <v>3</v>
+      </c>
+      <c r="G935">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="936" spans="1:7">
+      <c r="A936">
+        <v>2023</v>
+      </c>
+      <c r="B936">
+        <v>8</v>
+      </c>
+      <c r="C936">
+        <v>1</v>
+      </c>
+      <c r="D936" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E936">
+        <v>0.1</v>
+      </c>
+      <c r="F936">
+        <v>3</v>
+      </c>
+      <c r="G936">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="937" spans="1:7">
+      <c r="A937">
+        <v>2023</v>
+      </c>
+      <c r="B937">
+        <v>8</v>
+      </c>
+      <c r="C937">
+        <v>1</v>
+      </c>
+      <c r="D937" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E937">
+        <v>0.1</v>
+      </c>
+      <c r="F937">
+        <v>3</v>
+      </c>
+      <c r="G937">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="938" spans="1:7">
+      <c r="A938">
+        <v>2023</v>
+      </c>
+      <c r="B938">
+        <v>8</v>
+      </c>
+      <c r="C938">
+        <v>1</v>
+      </c>
+      <c r="D938" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E938">
+        <v>0.1</v>
+      </c>
+      <c r="F938">
+        <v>3</v>
+      </c>
+      <c r="G938">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="939" spans="1:7">
+      <c r="A939">
+        <v>2023</v>
+      </c>
+      <c r="B939">
+        <v>8</v>
+      </c>
+      <c r="C939">
+        <v>1</v>
+      </c>
+      <c r="D939" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E939">
+        <v>0.1</v>
+      </c>
+      <c r="F939">
+        <v>3</v>
+      </c>
+      <c r="G939">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="940" spans="1:7">
+      <c r="A940">
+        <v>2023</v>
+      </c>
+      <c r="B940">
+        <v>8</v>
+      </c>
+      <c r="C940">
+        <v>1</v>
+      </c>
+      <c r="D940" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E940">
+        <v>0.1</v>
+      </c>
+      <c r="F940">
+        <v>3</v>
+      </c>
+      <c r="G940">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="941" spans="1:7">
+      <c r="A941">
+        <v>2023</v>
+      </c>
+      <c r="B941">
+        <v>8</v>
+      </c>
+      <c r="C941">
+        <v>1</v>
+      </c>
+      <c r="D941" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E941">
+        <v>0.1</v>
+      </c>
+      <c r="F941">
+        <v>3</v>
+      </c>
+      <c r="G941">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="942" spans="1:7">
+      <c r="A942">
+        <v>2023</v>
+      </c>
+      <c r="B942">
+        <v>8</v>
+      </c>
+      <c r="C942">
+        <v>1</v>
+      </c>
+      <c r="D942" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E942">
+        <v>0.1</v>
+      </c>
+      <c r="F942">
+        <v>3</v>
+      </c>
+      <c r="G942">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="943" spans="1:7">
+      <c r="A943">
+        <v>2023</v>
+      </c>
+      <c r="B943">
+        <v>8</v>
+      </c>
+      <c r="C943">
+        <v>1</v>
+      </c>
+      <c r="D943" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E943">
+        <v>0.1</v>
+      </c>
+      <c r="F943">
+        <v>3</v>
+      </c>
+      <c r="G943">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="944" spans="1:7">
+      <c r="A944">
+        <v>2023</v>
+      </c>
+      <c r="B944">
+        <v>8</v>
+      </c>
+      <c r="C944">
+        <v>1</v>
+      </c>
+      <c r="D944" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E944">
+        <v>0.1</v>
+      </c>
+      <c r="F944">
+        <v>3</v>
+      </c>
+      <c r="G944">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="945" spans="1:7">
+      <c r="A945">
+        <v>2023</v>
+      </c>
+      <c r="B945">
+        <v>8</v>
+      </c>
+      <c r="C945">
+        <v>1</v>
+      </c>
+      <c r="D945" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E945">
+        <v>0.1</v>
+      </c>
+      <c r="F945">
+        <v>3</v>
+      </c>
+      <c r="G945">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="946" spans="1:7">
+      <c r="A946">
+        <v>2023</v>
+      </c>
+      <c r="B946">
+        <v>8</v>
+      </c>
+      <c r="C946">
+        <v>1</v>
+      </c>
+      <c r="D946" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E946">
+        <v>0.1</v>
+      </c>
+      <c r="F946">
+        <v>3</v>
+      </c>
+      <c r="G946">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="947" spans="1:7">
+      <c r="A947">
+        <v>2023</v>
+      </c>
+      <c r="B947">
+        <v>8</v>
+      </c>
+      <c r="C947">
+        <v>1</v>
+      </c>
+      <c r="D947" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E947">
+        <v>0.1</v>
+      </c>
+      <c r="F947">
+        <v>3</v>
+      </c>
+      <c r="G947">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="948" spans="1:7">
+      <c r="A948">
+        <v>2023</v>
+      </c>
+      <c r="B948">
+        <v>8</v>
+      </c>
+      <c r="C948">
+        <v>1</v>
+      </c>
+      <c r="D948" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E948">
+        <v>0.1</v>
+      </c>
+      <c r="F948">
+        <v>3</v>
+      </c>
+      <c r="G948">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="949" spans="1:7">
+      <c r="A949">
+        <v>2023</v>
+      </c>
+      <c r="B949">
+        <v>8</v>
+      </c>
+      <c r="C949">
+        <v>1</v>
+      </c>
+      <c r="D949" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E949">
+        <v>0.1</v>
+      </c>
+      <c r="F949">
+        <v>4</v>
+      </c>
+      <c r="G949">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="950" spans="1:7">
+      <c r="A950">
+        <v>2023</v>
+      </c>
+      <c r="B950">
+        <v>8</v>
+      </c>
+      <c r="C950">
+        <v>1</v>
+      </c>
+      <c r="D950" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E950">
+        <v>0.1</v>
+      </c>
+      <c r="F950">
+        <v>4</v>
+      </c>
+      <c r="G950">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="951" spans="1:7">
+      <c r="A951">
+        <v>2023</v>
+      </c>
+      <c r="B951">
+        <v>8</v>
+      </c>
+      <c r="C951">
+        <v>1</v>
+      </c>
+      <c r="D951" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E951">
+        <v>0.1</v>
+      </c>
+      <c r="F951">
+        <v>4</v>
+      </c>
+      <c r="G951">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="952" spans="1:7">
+      <c r="A952">
+        <v>2023</v>
+      </c>
+      <c r="B952">
+        <v>8</v>
+      </c>
+      <c r="C952">
+        <v>1</v>
+      </c>
+      <c r="D952" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E952">
+        <v>0.1</v>
+      </c>
+      <c r="F952">
+        <v>4</v>
+      </c>
+      <c r="G952">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="953" spans="1:7">
+      <c r="A953">
+        <v>2023</v>
+      </c>
+      <c r="B953">
+        <v>8</v>
+      </c>
+      <c r="C953">
+        <v>1</v>
+      </c>
+      <c r="D953" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E953">
+        <v>0.1</v>
+      </c>
+      <c r="F953">
+        <v>4</v>
+      </c>
+      <c r="G953">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="954" spans="1:7">
+      <c r="A954">
+        <v>2023</v>
+      </c>
+      <c r="B954">
+        <v>8</v>
+      </c>
+      <c r="C954">
+        <v>1</v>
+      </c>
+      <c r="D954" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E954">
+        <v>0.1</v>
+      </c>
+      <c r="F954">
+        <v>4</v>
+      </c>
+      <c r="G954">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="955" spans="1:7">
+      <c r="A955">
+        <v>2023</v>
+      </c>
+      <c r="B955">
+        <v>8</v>
+      </c>
+      <c r="C955">
+        <v>1</v>
+      </c>
+      <c r="D955" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E955">
+        <v>0.1</v>
+      </c>
+      <c r="F955">
+        <v>4</v>
+      </c>
+      <c r="G955">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="956" spans="1:7">
+      <c r="A956">
+        <v>2023</v>
+      </c>
+      <c r="B956">
+        <v>8</v>
+      </c>
+      <c r="C956">
+        <v>1</v>
+      </c>
+      <c r="D956" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E956">
+        <v>0.1</v>
+      </c>
+      <c r="F956">
+        <v>4</v>
+      </c>
+      <c r="G956">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="957" spans="1:7">
+      <c r="A957">
+        <v>2023</v>
+      </c>
+      <c r="B957">
+        <v>8</v>
+      </c>
+      <c r="C957">
+        <v>1</v>
+      </c>
+      <c r="D957" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E957">
+        <v>0.1</v>
+      </c>
+      <c r="F957">
+        <v>4</v>
+      </c>
+      <c r="G957">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="958" spans="1:7">
+      <c r="A958">
+        <v>2023</v>
+      </c>
+      <c r="B958">
+        <v>8</v>
+      </c>
+      <c r="C958">
+        <v>1</v>
+      </c>
+      <c r="D958" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E958">
+        <v>0.1</v>
+      </c>
+      <c r="F958">
+        <v>4</v>
+      </c>
+      <c r="G958">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="959" spans="1:7">
+      <c r="A959">
+        <v>2023</v>
+      </c>
+      <c r="B959">
+        <v>8</v>
+      </c>
+      <c r="C959">
+        <v>1</v>
+      </c>
+      <c r="D959" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E959">
+        <v>0.1</v>
+      </c>
+      <c r="F959">
+        <v>4</v>
+      </c>
+      <c r="G959">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="960" spans="1:7">
+      <c r="A960">
+        <v>2023</v>
+      </c>
+      <c r="B960">
+        <v>8</v>
+      </c>
+      <c r="C960">
+        <v>1</v>
+      </c>
+      <c r="D960" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E960">
+        <v>0.1</v>
+      </c>
+      <c r="F960">
+        <v>4</v>
+      </c>
+      <c r="G960">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="961" spans="1:7">
+      <c r="A961">
+        <v>2023</v>
+      </c>
+      <c r="B961">
+        <v>8</v>
+      </c>
+      <c r="C961">
+        <v>1</v>
+      </c>
+      <c r="D961" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E961">
+        <v>0.1</v>
+      </c>
+      <c r="F961">
+        <v>4</v>
+      </c>
+      <c r="G961">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="962" spans="1:7">
+      <c r="A962">
+        <v>2023</v>
+      </c>
+      <c r="B962">
+        <v>8</v>
+      </c>
+      <c r="C962">
+        <v>1</v>
+      </c>
+      <c r="D962" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E962">
+        <v>0.1</v>
+      </c>
+      <c r="F962">
+        <v>4</v>
+      </c>
+      <c r="G962">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="963" spans="1:7">
+      <c r="A963">
+        <v>2023</v>
+      </c>
+      <c r="B963">
+        <v>8</v>
+      </c>
+      <c r="C963">
+        <v>1</v>
+      </c>
+      <c r="D963" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E963">
+        <v>0.1</v>
+      </c>
+      <c r="F963">
+        <v>4</v>
+      </c>
+      <c r="G963">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="964" spans="1:7">
+      <c r="A964">
+        <v>2023</v>
+      </c>
+      <c r="B964">
+        <v>8</v>
+      </c>
+      <c r="C964">
+        <v>1</v>
+      </c>
+      <c r="D964" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E964">
+        <v>0.1</v>
+      </c>
+      <c r="F964">
+        <v>4</v>
+      </c>
+      <c r="G964">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="965" spans="1:7">
+      <c r="A965">
+        <v>2023</v>
+      </c>
+      <c r="B965">
+        <v>8</v>
+      </c>
+      <c r="C965">
+        <v>1</v>
+      </c>
+      <c r="D965" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E965">
+        <v>0.1</v>
+      </c>
+      <c r="F965">
+        <v>4</v>
+      </c>
+      <c r="G965">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="966" spans="1:7">
+      <c r="A966">
+        <v>2023</v>
+      </c>
+      <c r="B966">
+        <v>8</v>
+      </c>
+      <c r="C966">
+        <v>1</v>
+      </c>
+      <c r="D966" s="3">
+        <v>0.51111111111111096</v>
+      </c>
+      <c r="E966">
+        <v>0.1</v>
+      </c>
+      <c r="F966">
+        <v>4</v>
+      </c>
+      <c r="G966">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
functional form test and nov transects
</commit_message>
<xml_diff>
--- a/GW_seaweed_seasonality_transect_data.xlsx
+++ b/GW_seaweed_seasonality_transect_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1777" documentId="14_{436B2594-DD65-4C9F-B810-8D9ACA7BE4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED926601-E058-4135-B968-961BB5BB8738}"/>
+  <xr:revisionPtr revIDLastSave="2223" documentId="14_{436B2594-DD65-4C9F-B810-8D9ACA7BE4CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B711CA9E-FE06-4BD2-A454-292739F154AD}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="in" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">in!$A$1:$CI$1318</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">in!$A$1:$CK$1318</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1119" uniqueCount="130">
   <si>
     <t>year</t>
   </si>
@@ -420,6 +420,15 @@
   </si>
   <si>
     <t>snails-percentcover__invert</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>callithamnion_acutum__red</t>
+  </si>
+  <si>
+    <t>tiffaniella_snyderae__red</t>
   </si>
 </sst>
 </file>
@@ -1296,12 +1305,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CI1465"/>
+  <dimension ref="A1:CK1509"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1454" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1507" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AY1" sqref="AY1"/>
-      <selection pane="bottomLeft" activeCell="F1476" sqref="F1476"/>
+      <selection pane="bottomLeft" activeCell="K1524" sqref="K1524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1323,20 +1332,20 @@
     <col min="15" max="15" width="6.33203125" customWidth="1"/>
     <col min="16" max="16" width="7.44140625" customWidth="1"/>
     <col min="17" max="17" width="13.44140625" customWidth="1"/>
-    <col min="18" max="18" width="15.44140625" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="14" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="11.21875" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="10" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="9.44140625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="20" width="11.21875" customWidth="1"/>
+    <col min="21" max="21" width="10" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" customWidth="1"/>
     <col min="23" max="23" width="10.21875" customWidth="1"/>
     <col min="24" max="24" width="12.33203125" customWidth="1"/>
-    <col min="25" max="25" width="13" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="12.5546875" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="13.109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="5.6640625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="7.109375" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="5.6640625" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="4.109375" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="13" customWidth="1"/>
+    <col min="26" max="26" width="12.5546875" customWidth="1"/>
+    <col min="27" max="27" width="13.109375" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" customWidth="1"/>
+    <col min="29" max="29" width="7.109375" customWidth="1"/>
+    <col min="30" max="30" width="5.6640625" customWidth="1"/>
+    <col min="31" max="31" width="4.109375" customWidth="1"/>
     <col min="32" max="32" width="11.5546875" customWidth="1"/>
     <col min="33" max="34" width="8.88671875" hidden="1" customWidth="1"/>
     <col min="35" max="35" width="7.6640625" hidden="1" customWidth="1"/>
@@ -1384,11 +1393,11 @@
     <col min="79" max="79" width="4.109375" customWidth="1"/>
     <col min="80" max="83" width="5.88671875" customWidth="1"/>
     <col min="84" max="84" width="8.44140625" customWidth="1"/>
-    <col min="85" max="85" width="6.77734375" customWidth="1"/>
-    <col min="86" max="87" width="5" customWidth="1"/>
+    <col min="85" max="87" width="6.77734375" customWidth="1"/>
+    <col min="88" max="89" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1645,11 +1654,17 @@
         <v>118</v>
       </c>
       <c r="CH1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="CI1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="CJ1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="CI1" s="1"/>
-    </row>
-    <row r="2" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="CK1" s="1"/>
+    </row>
+    <row r="2" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2021</v>
       </c>
@@ -1684,7 +1699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -1713,7 +1728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -1742,7 +1757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2021</v>
       </c>
@@ -1774,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2021</v>
       </c>
@@ -1803,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2021</v>
       </c>
@@ -1832,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>2021</v>
       </c>
@@ -1870,7 +1885,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2021</v>
       </c>
@@ -1905,7 +1920,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>2021</v>
       </c>
@@ -1937,7 +1952,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -1969,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2021</v>
       </c>
@@ -2004,7 +2019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2021</v>
       </c>
@@ -2039,7 +2054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -2074,7 +2089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -2109,7 +2124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:87" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:89" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -24107,7 +24122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="593" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="593" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A593">
         <v>2023</v>
       </c>
@@ -24145,7 +24160,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="594" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="594" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A594">
         <v>2023</v>
       </c>
@@ -24183,7 +24198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="595" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="595" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A595">
         <v>2023</v>
       </c>
@@ -24227,7 +24242,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="596" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="596" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A596">
         <v>2023</v>
       </c>
@@ -24279,11 +24294,11 @@
       <c r="BY596">
         <v>5</v>
       </c>
-      <c r="CH596">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="597" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="CJ596">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="597" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A597">
         <v>2023</v>
       </c>
@@ -24321,7 +24336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="598" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="598" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A598">
         <v>2023</v>
       </c>
@@ -24356,7 +24371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="599" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="599" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A599">
         <v>2023</v>
       </c>
@@ -24400,7 +24415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="600" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="600" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A600">
         <v>2023</v>
       </c>
@@ -24438,7 +24453,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="601" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="601" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A601">
         <v>2023</v>
       </c>
@@ -24470,7 +24485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="602" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="602" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A602">
         <v>2023</v>
       </c>
@@ -24502,7 +24517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="603" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="603" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A603">
         <v>2023</v>
       </c>
@@ -24534,7 +24549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="604" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="604" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A604">
         <v>2023</v>
       </c>
@@ -24563,7 +24578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="605" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="605" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A605">
         <v>2023</v>
       </c>
@@ -24592,7 +24607,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="606" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="606" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A606">
         <v>2023</v>
       </c>
@@ -24621,7 +24636,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="607" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="607" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A607">
         <v>2023</v>
       </c>
@@ -24656,7 +24671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="608" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="608" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A608">
         <v>2023</v>
       </c>
@@ -34199,7 +34214,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="833" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="833" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A833">
         <v>2023</v>
       </c>
@@ -34237,7 +34252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="834" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="834" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A834">
         <v>2023</v>
       </c>
@@ -34278,7 +34293,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="835" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="835" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A835">
         <v>2023</v>
       </c>
@@ -34318,11 +34333,11 @@
       <c r="BI835">
         <v>1</v>
       </c>
-      <c r="CH835">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="836" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="CJ835">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="836" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A836">
         <v>2023</v>
       </c>
@@ -34372,7 +34387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="837" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="837" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A837">
         <v>2023</v>
       </c>
@@ -34425,7 +34440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="838" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="838" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A838">
         <v>2023</v>
       </c>
@@ -34466,7 +34481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="839" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="839" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A839">
         <v>2023</v>
       </c>
@@ -34504,7 +34519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="840" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="840" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A840">
         <v>2023</v>
       </c>
@@ -34545,7 +34560,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="841" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="841" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A841">
         <v>2023</v>
       </c>
@@ -34589,7 +34604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="842" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="842" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A842">
         <v>2023</v>
       </c>
@@ -34624,7 +34639,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="843" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="843" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A843">
         <v>2023</v>
       </c>
@@ -34662,7 +34677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="844" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="844" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A844">
         <v>2023</v>
       </c>
@@ -34700,7 +34715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="845" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="845" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A845">
         <v>2023</v>
       </c>
@@ -34738,7 +34753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="846" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="846" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A846">
         <v>2023</v>
       </c>
@@ -34776,7 +34791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="847" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="847" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A847">
         <v>2023</v>
       </c>
@@ -34811,7 +34826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="848" spans="1:86" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="848" spans="1:88" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A848">
         <v>2023</v>
       </c>
@@ -60456,6 +60471,2689 @@
       </c>
       <c r="AY1465">
         <v>3</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1466">
+        <v>2024</v>
+      </c>
+      <c r="B1466">
+        <v>11</v>
+      </c>
+      <c r="C1466">
+        <v>15</v>
+      </c>
+      <c r="D1466" s="3">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E1466">
+        <v>0.3</v>
+      </c>
+      <c r="F1466">
+        <v>2</v>
+      </c>
+      <c r="G1466">
+        <v>0</v>
+      </c>
+      <c r="I1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1466" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1466">
+        <v>1</v>
+      </c>
+      <c r="W1466">
+        <v>1</v>
+      </c>
+      <c r="AC1466">
+        <v>1</v>
+      </c>
+      <c r="AF1466">
+        <v>1</v>
+      </c>
+      <c r="AU1466">
+        <v>1</v>
+      </c>
+      <c r="AV1466">
+        <v>5</v>
+      </c>
+      <c r="AY1466">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1467">
+        <v>2024</v>
+      </c>
+      <c r="B1467">
+        <v>11</v>
+      </c>
+      <c r="C1467">
+        <v>15</v>
+      </c>
+      <c r="D1467" s="3">
+        <v>0.47569444444444442</v>
+      </c>
+      <c r="E1467">
+        <v>0.3</v>
+      </c>
+      <c r="F1467">
+        <v>2</v>
+      </c>
+      <c r="G1467">
+        <v>5</v>
+      </c>
+      <c r="I1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1467" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF1467">
+        <v>1</v>
+      </c>
+      <c r="AU1467">
+        <v>1</v>
+      </c>
+      <c r="AW1467">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1468">
+        <v>2024</v>
+      </c>
+      <c r="B1468">
+        <v>11</v>
+      </c>
+      <c r="C1468">
+        <v>15</v>
+      </c>
+      <c r="D1468" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1468">
+        <v>0.3</v>
+      </c>
+      <c r="F1468">
+        <v>2</v>
+      </c>
+      <c r="G1468">
+        <v>10</v>
+      </c>
+      <c r="I1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1468" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1468">
+        <v>2</v>
+      </c>
+      <c r="AF1468">
+        <v>50</v>
+      </c>
+      <c r="AU1468">
+        <v>1</v>
+      </c>
+      <c r="AV1468">
+        <v>5</v>
+      </c>
+      <c r="AW1468">
+        <v>30</v>
+      </c>
+      <c r="AY1468">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1469">
+        <v>2024</v>
+      </c>
+      <c r="B1469">
+        <v>11</v>
+      </c>
+      <c r="C1469">
+        <v>15</v>
+      </c>
+      <c r="D1469" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1469">
+        <v>0.3</v>
+      </c>
+      <c r="F1469">
+        <v>2</v>
+      </c>
+      <c r="G1469">
+        <v>15</v>
+      </c>
+      <c r="I1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1469" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1469">
+        <v>5</v>
+      </c>
+      <c r="W1469">
+        <v>1</v>
+      </c>
+      <c r="AF1469">
+        <v>1</v>
+      </c>
+      <c r="AU1469">
+        <v>1</v>
+      </c>
+      <c r="AW1469">
+        <v>5</v>
+      </c>
+      <c r="AY1469">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1470">
+        <v>2024</v>
+      </c>
+      <c r="B1470">
+        <v>11</v>
+      </c>
+      <c r="C1470">
+        <v>15</v>
+      </c>
+      <c r="D1470" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1470">
+        <v>0.3</v>
+      </c>
+      <c r="F1470">
+        <v>2</v>
+      </c>
+      <c r="G1470">
+        <v>20</v>
+      </c>
+      <c r="I1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1470" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1470">
+        <v>1</v>
+      </c>
+      <c r="AF1470">
+        <v>5</v>
+      </c>
+      <c r="AU1470">
+        <v>1</v>
+      </c>
+      <c r="AW1470">
+        <v>1</v>
+      </c>
+      <c r="BI1470">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1471">
+        <v>2024</v>
+      </c>
+      <c r="B1471">
+        <v>11</v>
+      </c>
+      <c r="C1471">
+        <v>15</v>
+      </c>
+      <c r="D1471" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1471">
+        <v>0.3</v>
+      </c>
+      <c r="F1471">
+        <v>2</v>
+      </c>
+      <c r="G1471">
+        <v>25</v>
+      </c>
+      <c r="I1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1471" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1471">
+        <v>10</v>
+      </c>
+      <c r="W1471">
+        <v>1</v>
+      </c>
+      <c r="AF1471">
+        <v>1</v>
+      </c>
+      <c r="AU1471">
+        <v>1</v>
+      </c>
+      <c r="AV1471">
+        <v>1</v>
+      </c>
+      <c r="AW1471">
+        <v>1</v>
+      </c>
+      <c r="AY1471">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:80" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1472">
+        <v>2024</v>
+      </c>
+      <c r="B1472">
+        <v>11</v>
+      </c>
+      <c r="C1472">
+        <v>15</v>
+      </c>
+      <c r="D1472" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1472">
+        <v>0.3</v>
+      </c>
+      <c r="F1472">
+        <v>2</v>
+      </c>
+      <c r="G1472">
+        <v>30</v>
+      </c>
+      <c r="I1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1472" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1472">
+        <v>1</v>
+      </c>
+      <c r="X1472">
+        <v>1</v>
+      </c>
+      <c r="AF1472">
+        <v>10</v>
+      </c>
+      <c r="AU1472">
+        <v>1</v>
+      </c>
+      <c r="AY1472">
+        <v>1</v>
+      </c>
+      <c r="AZ1472">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1473">
+        <v>2024</v>
+      </c>
+      <c r="B1473">
+        <v>11</v>
+      </c>
+      <c r="C1473">
+        <v>15</v>
+      </c>
+      <c r="D1473" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1473">
+        <v>0.3</v>
+      </c>
+      <c r="F1473">
+        <v>2</v>
+      </c>
+      <c r="G1473">
+        <v>35</v>
+      </c>
+      <c r="I1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1473" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1473">
+        <v>2</v>
+      </c>
+      <c r="AF1473">
+        <v>3</v>
+      </c>
+      <c r="AU1473">
+        <v>10</v>
+      </c>
+      <c r="AV1473">
+        <v>1</v>
+      </c>
+      <c r="AW1473">
+        <v>1</v>
+      </c>
+      <c r="BA1473">
+        <v>1</v>
+      </c>
+      <c r="BB1473">
+        <v>1</v>
+      </c>
+      <c r="BF1473">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1474">
+        <v>2024</v>
+      </c>
+      <c r="B1474">
+        <v>11</v>
+      </c>
+      <c r="C1474">
+        <v>15</v>
+      </c>
+      <c r="D1474" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1474">
+        <v>0.3</v>
+      </c>
+      <c r="F1474">
+        <v>2</v>
+      </c>
+      <c r="G1474">
+        <v>40</v>
+      </c>
+      <c r="I1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1474" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1474">
+        <v>5</v>
+      </c>
+      <c r="X1474">
+        <v>1</v>
+      </c>
+      <c r="AF1474">
+        <v>15</v>
+      </c>
+      <c r="AU1474">
+        <v>10</v>
+      </c>
+      <c r="AV1474">
+        <v>5</v>
+      </c>
+      <c r="AY1474">
+        <v>10</v>
+      </c>
+      <c r="BA1474">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1475">
+        <v>2024</v>
+      </c>
+      <c r="B1475">
+        <v>11</v>
+      </c>
+      <c r="C1475">
+        <v>15</v>
+      </c>
+      <c r="D1475" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1475">
+        <v>0.3</v>
+      </c>
+      <c r="F1475">
+        <v>3</v>
+      </c>
+      <c r="G1475">
+        <v>0</v>
+      </c>
+      <c r="I1475">
+        <v>500</v>
+      </c>
+      <c r="K1475">
+        <v>50</v>
+      </c>
+      <c r="L1475">
+        <v>10</v>
+      </c>
+      <c r="M1475">
+        <v>100</v>
+      </c>
+      <c r="Q1475">
+        <v>20</v>
+      </c>
+      <c r="W1475">
+        <v>1</v>
+      </c>
+      <c r="AC1475">
+        <v>1</v>
+      </c>
+      <c r="AF1475">
+        <v>5</v>
+      </c>
+      <c r="AU1475">
+        <v>3</v>
+      </c>
+      <c r="AV1475">
+        <v>10</v>
+      </c>
+      <c r="AW1475">
+        <v>1</v>
+      </c>
+      <c r="AY1475">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1476">
+        <v>2024</v>
+      </c>
+      <c r="B1476">
+        <v>11</v>
+      </c>
+      <c r="C1476">
+        <v>15</v>
+      </c>
+      <c r="D1476" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1476">
+        <v>0.3</v>
+      </c>
+      <c r="F1476">
+        <v>3</v>
+      </c>
+      <c r="G1476">
+        <v>5</v>
+      </c>
+      <c r="I1476" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1476">
+        <v>5</v>
+      </c>
+      <c r="K1476">
+        <v>30</v>
+      </c>
+      <c r="L1476">
+        <v>5</v>
+      </c>
+      <c r="N1476">
+        <v>80</v>
+      </c>
+      <c r="O1476">
+        <v>20</v>
+      </c>
+      <c r="AF1476">
+        <v>3</v>
+      </c>
+      <c r="AU1476">
+        <v>1</v>
+      </c>
+      <c r="AW1476">
+        <v>5</v>
+      </c>
+      <c r="AY1476">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1477">
+        <v>2024</v>
+      </c>
+      <c r="B1477">
+        <v>11</v>
+      </c>
+      <c r="C1477">
+        <v>15</v>
+      </c>
+      <c r="D1477" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1477">
+        <v>0.3</v>
+      </c>
+      <c r="F1477">
+        <v>3</v>
+      </c>
+      <c r="G1477">
+        <v>10</v>
+      </c>
+      <c r="I1477" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1477">
+        <v>5</v>
+      </c>
+      <c r="K1477">
+        <v>70</v>
+      </c>
+      <c r="L1477">
+        <v>200</v>
+      </c>
+      <c r="M1477">
+        <v>80</v>
+      </c>
+      <c r="N1477">
+        <v>15</v>
+      </c>
+      <c r="O1477">
+        <v>5</v>
+      </c>
+      <c r="Q1477">
+        <v>1</v>
+      </c>
+      <c r="W1477">
+        <v>1</v>
+      </c>
+      <c r="AF1477">
+        <v>10</v>
+      </c>
+      <c r="AU1477">
+        <v>1</v>
+      </c>
+      <c r="AV1477">
+        <v>1</v>
+      </c>
+      <c r="AW1477">
+        <v>5</v>
+      </c>
+      <c r="AY1477">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1478">
+        <v>2024</v>
+      </c>
+      <c r="B1478">
+        <v>11</v>
+      </c>
+      <c r="C1478">
+        <v>15</v>
+      </c>
+      <c r="D1478" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1478">
+        <v>0.3</v>
+      </c>
+      <c r="F1478">
+        <v>3</v>
+      </c>
+      <c r="G1478">
+        <v>15</v>
+      </c>
+      <c r="I1478" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1478">
+        <v>2</v>
+      </c>
+      <c r="K1478">
+        <v>30</v>
+      </c>
+      <c r="L1478">
+        <v>100</v>
+      </c>
+      <c r="M1478">
+        <v>15</v>
+      </c>
+      <c r="N1478">
+        <v>70</v>
+      </c>
+      <c r="O1478">
+        <v>15</v>
+      </c>
+      <c r="W1478">
+        <v>1</v>
+      </c>
+      <c r="AF1478">
+        <v>2</v>
+      </c>
+      <c r="AU1478">
+        <v>1</v>
+      </c>
+      <c r="AW1478">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1479">
+        <v>2024</v>
+      </c>
+      <c r="B1479">
+        <v>11</v>
+      </c>
+      <c r="C1479">
+        <v>15</v>
+      </c>
+      <c r="D1479" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1479">
+        <v>0.3</v>
+      </c>
+      <c r="F1479">
+        <v>3</v>
+      </c>
+      <c r="G1479">
+        <v>20</v>
+      </c>
+      <c r="I1479" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1479">
+        <v>5</v>
+      </c>
+      <c r="K1479">
+        <v>10</v>
+      </c>
+      <c r="L1479">
+        <v>50</v>
+      </c>
+      <c r="M1479">
+        <v>10</v>
+      </c>
+      <c r="N1479">
+        <v>80</v>
+      </c>
+      <c r="O1479">
+        <v>10</v>
+      </c>
+      <c r="Q1479">
+        <v>1</v>
+      </c>
+      <c r="AF1479">
+        <v>3</v>
+      </c>
+      <c r="AU1479">
+        <v>1</v>
+      </c>
+      <c r="AW1479">
+        <v>1</v>
+      </c>
+      <c r="AY1479">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1480">
+        <v>2024</v>
+      </c>
+      <c r="B1480">
+        <v>11</v>
+      </c>
+      <c r="C1480">
+        <v>15</v>
+      </c>
+      <c r="D1480" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1480">
+        <v>0.3</v>
+      </c>
+      <c r="F1480">
+        <v>3</v>
+      </c>
+      <c r="G1480">
+        <v>25</v>
+      </c>
+      <c r="I1480" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1480">
+        <v>1</v>
+      </c>
+      <c r="K1480">
+        <v>2</v>
+      </c>
+      <c r="N1480">
+        <v>60</v>
+      </c>
+      <c r="O1480">
+        <v>40</v>
+      </c>
+      <c r="X1480">
+        <v>1</v>
+      </c>
+      <c r="AF1480">
+        <v>4</v>
+      </c>
+      <c r="AY1480">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1481">
+        <v>2024</v>
+      </c>
+      <c r="B1481">
+        <v>11</v>
+      </c>
+      <c r="C1481">
+        <v>15</v>
+      </c>
+      <c r="D1481" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1481">
+        <v>0.3</v>
+      </c>
+      <c r="F1481">
+        <v>3</v>
+      </c>
+      <c r="G1481">
+        <v>30</v>
+      </c>
+      <c r="I1481" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1481">
+        <v>1</v>
+      </c>
+      <c r="K1481">
+        <v>5</v>
+      </c>
+      <c r="L1481">
+        <v>10</v>
+      </c>
+      <c r="M1481">
+        <v>20</v>
+      </c>
+      <c r="N1481">
+        <v>40</v>
+      </c>
+      <c r="O1481">
+        <v>40</v>
+      </c>
+      <c r="W1481">
+        <v>1</v>
+      </c>
+      <c r="AF1481">
+        <v>4</v>
+      </c>
+      <c r="AU1481">
+        <v>1</v>
+      </c>
+      <c r="AY1481">
+        <v>2</v>
+      </c>
+      <c r="BE1481">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1482">
+        <v>2024</v>
+      </c>
+      <c r="B1482">
+        <v>11</v>
+      </c>
+      <c r="C1482">
+        <v>15</v>
+      </c>
+      <c r="D1482" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1482">
+        <v>0.3</v>
+      </c>
+      <c r="F1482">
+        <v>3</v>
+      </c>
+      <c r="G1482">
+        <v>35</v>
+      </c>
+      <c r="I1482" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1482">
+        <v>1</v>
+      </c>
+      <c r="K1482">
+        <v>30</v>
+      </c>
+      <c r="N1482">
+        <v>80</v>
+      </c>
+      <c r="O1482">
+        <v>20</v>
+      </c>
+      <c r="Q1482">
+        <v>1</v>
+      </c>
+      <c r="AF1482">
+        <v>1</v>
+      </c>
+      <c r="AU1482">
+        <v>1</v>
+      </c>
+      <c r="AY1482">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1483">
+        <v>2024</v>
+      </c>
+      <c r="B1483">
+        <v>11</v>
+      </c>
+      <c r="C1483">
+        <v>15</v>
+      </c>
+      <c r="D1483" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1483">
+        <v>0.3</v>
+      </c>
+      <c r="F1483">
+        <v>3</v>
+      </c>
+      <c r="G1483">
+        <v>40</v>
+      </c>
+      <c r="I1483" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1483">
+        <v>10</v>
+      </c>
+      <c r="N1483">
+        <v>80</v>
+      </c>
+      <c r="O1483">
+        <v>20</v>
+      </c>
+      <c r="AF1483">
+        <v>3</v>
+      </c>
+      <c r="AU1483">
+        <v>1</v>
+      </c>
+      <c r="AY1483">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1484">
+        <v>2024</v>
+      </c>
+      <c r="B1484">
+        <v>11</v>
+      </c>
+      <c r="C1484">
+        <v>15</v>
+      </c>
+      <c r="D1484" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1484">
+        <v>0.3</v>
+      </c>
+      <c r="F1484">
+        <v>3</v>
+      </c>
+      <c r="G1484">
+        <v>45</v>
+      </c>
+      <c r="I1484" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1484">
+        <v>20</v>
+      </c>
+      <c r="M1484">
+        <v>15</v>
+      </c>
+      <c r="N1484">
+        <v>75</v>
+      </c>
+      <c r="O1484">
+        <v>10</v>
+      </c>
+      <c r="Q1484">
+        <v>1</v>
+      </c>
+      <c r="X1484">
+        <v>1</v>
+      </c>
+      <c r="AF1484">
+        <v>10</v>
+      </c>
+      <c r="AU1484">
+        <v>3</v>
+      </c>
+      <c r="AY1484">
+        <v>15</v>
+      </c>
+      <c r="BA1484">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1485">
+        <v>2024</v>
+      </c>
+      <c r="B1485">
+        <v>11</v>
+      </c>
+      <c r="C1485">
+        <v>15</v>
+      </c>
+      <c r="D1485" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1485">
+        <v>0.3</v>
+      </c>
+      <c r="F1485">
+        <v>3</v>
+      </c>
+      <c r="G1485">
+        <v>50</v>
+      </c>
+      <c r="I1485" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1485">
+        <v>5</v>
+      </c>
+      <c r="M1485">
+        <v>5</v>
+      </c>
+      <c r="N1485">
+        <v>90</v>
+      </c>
+      <c r="O1485">
+        <v>5</v>
+      </c>
+      <c r="Q1485">
+        <v>1</v>
+      </c>
+      <c r="W1485">
+        <v>1</v>
+      </c>
+      <c r="X1485">
+        <v>1</v>
+      </c>
+      <c r="AF1485">
+        <v>10</v>
+      </c>
+      <c r="AU1485">
+        <v>2</v>
+      </c>
+      <c r="AW1485">
+        <v>1</v>
+      </c>
+      <c r="AY1485">
+        <v>20</v>
+      </c>
+      <c r="BA1485">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1486">
+        <v>2024</v>
+      </c>
+      <c r="B1486">
+        <v>11</v>
+      </c>
+      <c r="C1486">
+        <v>15</v>
+      </c>
+      <c r="D1486" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1486">
+        <v>0.3</v>
+      </c>
+      <c r="F1486">
+        <v>3</v>
+      </c>
+      <c r="G1486">
+        <v>55</v>
+      </c>
+      <c r="I1486" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1486">
+        <v>5</v>
+      </c>
+      <c r="M1486">
+        <v>10</v>
+      </c>
+      <c r="N1486">
+        <v>90</v>
+      </c>
+      <c r="Q1486">
+        <v>1</v>
+      </c>
+      <c r="AF1486">
+        <v>15</v>
+      </c>
+      <c r="AU1486">
+        <v>5</v>
+      </c>
+      <c r="AY1486">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1487">
+        <v>2024</v>
+      </c>
+      <c r="B1487">
+        <v>11</v>
+      </c>
+      <c r="C1487">
+        <v>15</v>
+      </c>
+      <c r="D1487" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1487">
+        <v>0.3</v>
+      </c>
+      <c r="F1487">
+        <v>3</v>
+      </c>
+      <c r="G1487">
+        <v>60</v>
+      </c>
+      <c r="I1487" t="s">
+        <v>127</v>
+      </c>
+      <c r="X1487">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1488">
+        <v>2024</v>
+      </c>
+      <c r="B1488">
+        <v>11</v>
+      </c>
+      <c r="C1488">
+        <v>15</v>
+      </c>
+      <c r="D1488" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1488">
+        <v>0.3</v>
+      </c>
+      <c r="F1488">
+        <v>3</v>
+      </c>
+      <c r="G1488">
+        <v>65</v>
+      </c>
+      <c r="I1488" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1488">
+        <v>5</v>
+      </c>
+      <c r="N1488">
+        <v>100</v>
+      </c>
+      <c r="AF1488">
+        <v>20</v>
+      </c>
+      <c r="AU1488">
+        <v>1</v>
+      </c>
+      <c r="AY1488">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1489">
+        <v>2024</v>
+      </c>
+      <c r="B1489">
+        <v>11</v>
+      </c>
+      <c r="C1489">
+        <v>15</v>
+      </c>
+      <c r="D1489" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1489">
+        <v>0.3</v>
+      </c>
+      <c r="F1489">
+        <v>3</v>
+      </c>
+      <c r="G1489">
+        <v>70</v>
+      </c>
+      <c r="I1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1489" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1489">
+        <v>2</v>
+      </c>
+      <c r="S1489">
+        <v>1</v>
+      </c>
+      <c r="X1489">
+        <v>5</v>
+      </c>
+      <c r="AF1489">
+        <v>30</v>
+      </c>
+      <c r="AU1489">
+        <v>1</v>
+      </c>
+      <c r="AV1489">
+        <v>1</v>
+      </c>
+      <c r="AY1489">
+        <v>10</v>
+      </c>
+      <c r="BE1489">
+        <v>1</v>
+      </c>
+      <c r="BN1489">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1490">
+        <v>2024</v>
+      </c>
+      <c r="B1490">
+        <v>11</v>
+      </c>
+      <c r="C1490">
+        <v>15</v>
+      </c>
+      <c r="D1490" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1490">
+        <v>0.3</v>
+      </c>
+      <c r="F1490">
+        <v>3</v>
+      </c>
+      <c r="G1490">
+        <v>75</v>
+      </c>
+      <c r="I1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1490" t="s">
+        <v>127</v>
+      </c>
+      <c r="X1490">
+        <v>1</v>
+      </c>
+      <c r="AF1490">
+        <v>20</v>
+      </c>
+      <c r="AU1490">
+        <v>5</v>
+      </c>
+      <c r="AY1490">
+        <v>40</v>
+      </c>
+      <c r="BC1490">
+        <v>1</v>
+      </c>
+      <c r="BE1490">
+        <v>1</v>
+      </c>
+      <c r="BZ1490">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1491">
+        <v>2024</v>
+      </c>
+      <c r="B1491">
+        <v>11</v>
+      </c>
+      <c r="C1491">
+        <v>15</v>
+      </c>
+      <c r="D1491" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1491">
+        <v>0.3</v>
+      </c>
+      <c r="F1491">
+        <v>3</v>
+      </c>
+      <c r="G1491">
+        <v>80</v>
+      </c>
+      <c r="I1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1491" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1491">
+        <v>2</v>
+      </c>
+      <c r="R1491">
+        <v>5</v>
+      </c>
+      <c r="W1491">
+        <v>1</v>
+      </c>
+      <c r="X1491">
+        <v>5</v>
+      </c>
+      <c r="AF1491">
+        <v>40</v>
+      </c>
+      <c r="AU1491">
+        <v>5</v>
+      </c>
+      <c r="AY1491">
+        <v>25</v>
+      </c>
+      <c r="AZ1491">
+        <v>5</v>
+      </c>
+      <c r="BA1491">
+        <v>10</v>
+      </c>
+      <c r="BE1491">
+        <v>2</v>
+      </c>
+      <c r="BF1491">
+        <v>1</v>
+      </c>
+      <c r="BZ1491">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1492">
+        <v>2024</v>
+      </c>
+      <c r="B1492">
+        <v>11</v>
+      </c>
+      <c r="C1492">
+        <v>15</v>
+      </c>
+      <c r="D1492" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1492">
+        <v>0.3</v>
+      </c>
+      <c r="F1492">
+        <v>3</v>
+      </c>
+      <c r="G1492">
+        <v>85</v>
+      </c>
+      <c r="I1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1492" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1492">
+        <v>1</v>
+      </c>
+      <c r="R1492">
+        <v>50</v>
+      </c>
+      <c r="X1492">
+        <v>2</v>
+      </c>
+      <c r="AF1492">
+        <v>30</v>
+      </c>
+      <c r="AU1492">
+        <v>20</v>
+      </c>
+      <c r="AV1492">
+        <v>5</v>
+      </c>
+      <c r="AY1492">
+        <v>20</v>
+      </c>
+      <c r="AZ1492">
+        <v>5</v>
+      </c>
+      <c r="BA1492">
+        <v>1</v>
+      </c>
+      <c r="BD1492">
+        <v>5</v>
+      </c>
+      <c r="BE1492">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1493">
+        <v>2024</v>
+      </c>
+      <c r="B1493">
+        <v>11</v>
+      </c>
+      <c r="C1493">
+        <v>15</v>
+      </c>
+      <c r="D1493" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1493">
+        <v>0.3</v>
+      </c>
+      <c r="F1493">
+        <v>3</v>
+      </c>
+      <c r="G1493">
+        <v>90</v>
+      </c>
+      <c r="I1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1493" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q1493">
+        <v>15</v>
+      </c>
+      <c r="R1493">
+        <v>30</v>
+      </c>
+      <c r="X1493">
+        <v>1</v>
+      </c>
+      <c r="AF1493">
+        <v>10</v>
+      </c>
+      <c r="AU1493">
+        <v>30</v>
+      </c>
+      <c r="AY1493">
+        <v>50</v>
+      </c>
+      <c r="AZ1493">
+        <v>5</v>
+      </c>
+      <c r="BD1493">
+        <v>1</v>
+      </c>
+      <c r="BE1493">
+        <v>1</v>
+      </c>
+      <c r="BF1493">
+        <v>1</v>
+      </c>
+      <c r="BG1493">
+        <v>1</v>
+      </c>
+      <c r="BN1493">
+        <v>1</v>
+      </c>
+      <c r="BS1493">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1494">
+        <v>2024</v>
+      </c>
+      <c r="B1494">
+        <v>11</v>
+      </c>
+      <c r="C1494">
+        <v>15</v>
+      </c>
+      <c r="D1494" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1494">
+        <v>0.3</v>
+      </c>
+      <c r="F1494">
+        <v>4</v>
+      </c>
+      <c r="G1494">
+        <v>0</v>
+      </c>
+      <c r="I1494">
+        <v>400</v>
+      </c>
+      <c r="J1494">
+        <v>5</v>
+      </c>
+      <c r="K1494">
+        <v>75</v>
+      </c>
+      <c r="L1494">
+        <v>22</v>
+      </c>
+      <c r="M1494">
+        <v>100</v>
+      </c>
+      <c r="Q1494">
+        <v>10</v>
+      </c>
+      <c r="W1494">
+        <v>2</v>
+      </c>
+      <c r="AC1494">
+        <v>1</v>
+      </c>
+      <c r="AF1494">
+        <v>5</v>
+      </c>
+      <c r="AU1494">
+        <v>3</v>
+      </c>
+      <c r="AV1494">
+        <v>4</v>
+      </c>
+      <c r="AW1494">
+        <v>1</v>
+      </c>
+      <c r="AY1494">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1495">
+        <v>2024</v>
+      </c>
+      <c r="B1495">
+        <v>11</v>
+      </c>
+      <c r="C1495">
+        <v>15</v>
+      </c>
+      <c r="D1495" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1495">
+        <v>0.3</v>
+      </c>
+      <c r="F1495">
+        <v>4</v>
+      </c>
+      <c r="G1495">
+        <v>5</v>
+      </c>
+      <c r="I1495" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1495">
+        <v>1</v>
+      </c>
+      <c r="K1495">
+        <v>40</v>
+      </c>
+      <c r="M1495">
+        <v>20</v>
+      </c>
+      <c r="N1495">
+        <v>30</v>
+      </c>
+      <c r="O1495">
+        <v>60</v>
+      </c>
+      <c r="AF1495">
+        <v>2</v>
+      </c>
+      <c r="AU1495">
+        <v>2</v>
+      </c>
+      <c r="AV1495">
+        <v>1</v>
+      </c>
+      <c r="AW1495">
+        <v>1</v>
+      </c>
+      <c r="AY1495">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1496">
+        <v>2024</v>
+      </c>
+      <c r="B1496">
+        <v>11</v>
+      </c>
+      <c r="C1496">
+        <v>15</v>
+      </c>
+      <c r="D1496" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1496">
+        <v>0.3</v>
+      </c>
+      <c r="F1496">
+        <v>4</v>
+      </c>
+      <c r="G1496">
+        <v>10</v>
+      </c>
+      <c r="I1496" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1496">
+        <v>2</v>
+      </c>
+      <c r="K1496">
+        <v>70</v>
+      </c>
+      <c r="L1496">
+        <v>1</v>
+      </c>
+      <c r="M1496">
+        <v>40</v>
+      </c>
+      <c r="N1496">
+        <v>30</v>
+      </c>
+      <c r="O1496">
+        <v>30</v>
+      </c>
+      <c r="AF1496">
+        <v>3</v>
+      </c>
+      <c r="AU1496">
+        <v>2</v>
+      </c>
+      <c r="AW1496">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1497">
+        <v>2024</v>
+      </c>
+      <c r="B1497">
+        <v>11</v>
+      </c>
+      <c r="C1497">
+        <v>15</v>
+      </c>
+      <c r="D1497" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1497">
+        <v>0.3</v>
+      </c>
+      <c r="F1497">
+        <v>4</v>
+      </c>
+      <c r="G1497">
+        <v>15</v>
+      </c>
+      <c r="I1497" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1497">
+        <v>2</v>
+      </c>
+      <c r="K1497">
+        <v>50</v>
+      </c>
+      <c r="L1497">
+        <v>8</v>
+      </c>
+      <c r="M1497">
+        <v>70</v>
+      </c>
+      <c r="N1497">
+        <v>10</v>
+      </c>
+      <c r="O1497">
+        <v>20</v>
+      </c>
+      <c r="AF1497">
+        <v>1</v>
+      </c>
+      <c r="AU1497">
+        <v>2</v>
+      </c>
+      <c r="AW1497">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1498">
+        <v>2024</v>
+      </c>
+      <c r="B1498">
+        <v>11</v>
+      </c>
+      <c r="C1498">
+        <v>15</v>
+      </c>
+      <c r="D1498" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1498">
+        <v>0.3</v>
+      </c>
+      <c r="F1498">
+        <v>4</v>
+      </c>
+      <c r="G1498">
+        <v>20</v>
+      </c>
+      <c r="I1498" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1498">
+        <v>2</v>
+      </c>
+      <c r="K1498">
+        <v>25</v>
+      </c>
+      <c r="L1498">
+        <v>7</v>
+      </c>
+      <c r="M1498">
+        <v>5</v>
+      </c>
+      <c r="N1498">
+        <v>45</v>
+      </c>
+      <c r="O1498">
+        <v>50</v>
+      </c>
+      <c r="Q1498">
+        <v>1</v>
+      </c>
+      <c r="W1498">
+        <v>1</v>
+      </c>
+      <c r="AF1498">
+        <v>1</v>
+      </c>
+      <c r="AU1498">
+        <v>1</v>
+      </c>
+      <c r="AY1498">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1499">
+        <v>2024</v>
+      </c>
+      <c r="B1499">
+        <v>11</v>
+      </c>
+      <c r="C1499">
+        <v>15</v>
+      </c>
+      <c r="D1499" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1499">
+        <v>0.3</v>
+      </c>
+      <c r="F1499">
+        <v>4</v>
+      </c>
+      <c r="G1499">
+        <v>25</v>
+      </c>
+      <c r="I1499" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1499">
+        <v>5</v>
+      </c>
+      <c r="K1499">
+        <v>25</v>
+      </c>
+      <c r="M1499">
+        <v>25</v>
+      </c>
+      <c r="N1499">
+        <v>35</v>
+      </c>
+      <c r="O1499">
+        <v>40</v>
+      </c>
+      <c r="AF1499">
+        <v>3</v>
+      </c>
+      <c r="AU1499">
+        <v>1</v>
+      </c>
+      <c r="AY1499">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1500">
+        <v>2024</v>
+      </c>
+      <c r="B1500">
+        <v>11</v>
+      </c>
+      <c r="C1500">
+        <v>15</v>
+      </c>
+      <c r="D1500" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1500">
+        <v>0.3</v>
+      </c>
+      <c r="F1500">
+        <v>4</v>
+      </c>
+      <c r="G1500">
+        <v>30</v>
+      </c>
+      <c r="I1500" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1500">
+        <v>1</v>
+      </c>
+      <c r="K1500">
+        <v>5</v>
+      </c>
+      <c r="L1500">
+        <v>2</v>
+      </c>
+      <c r="M1500">
+        <v>10</v>
+      </c>
+      <c r="N1500">
+        <v>40</v>
+      </c>
+      <c r="O1500">
+        <v>50</v>
+      </c>
+      <c r="AF1500">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1501">
+        <v>2024</v>
+      </c>
+      <c r="B1501">
+        <v>11</v>
+      </c>
+      <c r="C1501">
+        <v>15</v>
+      </c>
+      <c r="D1501" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1501">
+        <v>0.3</v>
+      </c>
+      <c r="F1501">
+        <v>4</v>
+      </c>
+      <c r="G1501">
+        <v>35</v>
+      </c>
+      <c r="I1501" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1501">
+        <v>1</v>
+      </c>
+      <c r="K1501">
+        <v>10</v>
+      </c>
+      <c r="L1501">
+        <v>2</v>
+      </c>
+      <c r="M1501">
+        <v>15</v>
+      </c>
+      <c r="N1501">
+        <v>30</v>
+      </c>
+      <c r="O1501">
+        <v>55</v>
+      </c>
+      <c r="P1501">
+        <v>10</v>
+      </c>
+      <c r="Q1501">
+        <v>1</v>
+      </c>
+      <c r="AF1501">
+        <v>20</v>
+      </c>
+      <c r="AU1501">
+        <v>1</v>
+      </c>
+      <c r="AY1501">
+        <v>1</v>
+      </c>
+      <c r="BC1501">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1502">
+        <v>2024</v>
+      </c>
+      <c r="B1502">
+        <v>11</v>
+      </c>
+      <c r="C1502">
+        <v>15</v>
+      </c>
+      <c r="D1502" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1502">
+        <v>0.3</v>
+      </c>
+      <c r="F1502">
+        <v>4</v>
+      </c>
+      <c r="G1502">
+        <v>40</v>
+      </c>
+      <c r="I1502" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1502">
+        <v>1</v>
+      </c>
+      <c r="K1502">
+        <v>5</v>
+      </c>
+      <c r="M1502">
+        <v>25</v>
+      </c>
+      <c r="N1502">
+        <v>30</v>
+      </c>
+      <c r="O1502">
+        <v>45</v>
+      </c>
+      <c r="P1502">
+        <v>10</v>
+      </c>
+      <c r="X1502">
+        <v>1</v>
+      </c>
+      <c r="AF1502">
+        <v>10</v>
+      </c>
+      <c r="AV1502">
+        <v>2</v>
+      </c>
+      <c r="CH1502">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1503">
+        <v>2024</v>
+      </c>
+      <c r="B1503">
+        <v>11</v>
+      </c>
+      <c r="C1503">
+        <v>15</v>
+      </c>
+      <c r="D1503" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1503">
+        <v>0.3</v>
+      </c>
+      <c r="F1503">
+        <v>4</v>
+      </c>
+      <c r="G1503">
+        <v>45</v>
+      </c>
+      <c r="I1503" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1503">
+        <v>1</v>
+      </c>
+      <c r="K1503">
+        <v>30</v>
+      </c>
+      <c r="M1503">
+        <v>30</v>
+      </c>
+      <c r="N1503">
+        <v>25</v>
+      </c>
+      <c r="O1503">
+        <v>25</v>
+      </c>
+      <c r="P1503">
+        <v>5</v>
+      </c>
+      <c r="X1503">
+        <v>1</v>
+      </c>
+      <c r="AF1503">
+        <v>30</v>
+      </c>
+      <c r="AU1503">
+        <v>2</v>
+      </c>
+      <c r="AV1503">
+        <v>4</v>
+      </c>
+      <c r="AY1503">
+        <v>5</v>
+      </c>
+      <c r="BI1503">
+        <v>1</v>
+      </c>
+      <c r="BJ1503">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:86" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1504">
+        <v>2024</v>
+      </c>
+      <c r="B1504">
+        <v>11</v>
+      </c>
+      <c r="C1504">
+        <v>15</v>
+      </c>
+      <c r="D1504" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1504">
+        <v>0.3</v>
+      </c>
+      <c r="F1504">
+        <v>4</v>
+      </c>
+      <c r="G1504">
+        <v>50</v>
+      </c>
+      <c r="I1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1504" t="s">
+        <v>127</v>
+      </c>
+      <c r="X1504">
+        <v>1</v>
+      </c>
+      <c r="AF1504">
+        <v>20</v>
+      </c>
+      <c r="AU1504">
+        <v>3</v>
+      </c>
+      <c r="AV1504">
+        <v>5</v>
+      </c>
+      <c r="AY1504">
+        <v>1</v>
+      </c>
+      <c r="AZ1504">
+        <v>1</v>
+      </c>
+      <c r="BD1504">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:87" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1505">
+        <v>2024</v>
+      </c>
+      <c r="B1505">
+        <v>11</v>
+      </c>
+      <c r="C1505">
+        <v>15</v>
+      </c>
+      <c r="D1505" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1505">
+        <v>0.3</v>
+      </c>
+      <c r="F1505">
+        <v>4</v>
+      </c>
+      <c r="G1505">
+        <v>55</v>
+      </c>
+      <c r="I1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1505" t="s">
+        <v>127</v>
+      </c>
+      <c r="X1505">
+        <v>3</v>
+      </c>
+      <c r="AF1505">
+        <v>40</v>
+      </c>
+      <c r="AV1505">
+        <v>3</v>
+      </c>
+      <c r="AY1505">
+        <v>1</v>
+      </c>
+      <c r="BD1505">
+        <v>1</v>
+      </c>
+      <c r="BE1505">
+        <v>1</v>
+      </c>
+      <c r="CI1505">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:87" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1506">
+        <v>2024</v>
+      </c>
+      <c r="B1506">
+        <v>11</v>
+      </c>
+      <c r="C1506">
+        <v>15</v>
+      </c>
+      <c r="D1506" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1506">
+        <v>0.3</v>
+      </c>
+      <c r="F1506">
+        <v>4</v>
+      </c>
+      <c r="G1506">
+        <v>60</v>
+      </c>
+      <c r="I1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1506" t="s">
+        <v>127</v>
+      </c>
+      <c r="X1506">
+        <v>1</v>
+      </c>
+      <c r="AF1506">
+        <v>40</v>
+      </c>
+      <c r="AU1506">
+        <v>5</v>
+      </c>
+      <c r="AV1506">
+        <v>3</v>
+      </c>
+      <c r="BD1506">
+        <v>1</v>
+      </c>
+      <c r="BE1506">
+        <v>1</v>
+      </c>
+      <c r="BJ1506">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:87" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1507">
+        <v>2024</v>
+      </c>
+      <c r="B1507">
+        <v>11</v>
+      </c>
+      <c r="C1507">
+        <v>15</v>
+      </c>
+      <c r="D1507" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1507">
+        <v>0.3</v>
+      </c>
+      <c r="F1507">
+        <v>4</v>
+      </c>
+      <c r="G1507">
+        <v>65</v>
+      </c>
+      <c r="I1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1507" t="s">
+        <v>127</v>
+      </c>
+      <c r="X1507">
+        <v>5</v>
+      </c>
+      <c r="AF1507">
+        <v>10</v>
+      </c>
+      <c r="BA1507">
+        <v>2</v>
+      </c>
+      <c r="BE1507">
+        <v>3</v>
+      </c>
+      <c r="BG1507">
+        <v>1</v>
+      </c>
+      <c r="BJ1507">
+        <v>1</v>
+      </c>
+      <c r="BW1507">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:87" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1508">
+        <v>2024</v>
+      </c>
+      <c r="B1508">
+        <v>11</v>
+      </c>
+      <c r="C1508">
+        <v>15</v>
+      </c>
+      <c r="D1508" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1508">
+        <v>0.3</v>
+      </c>
+      <c r="F1508">
+        <v>4</v>
+      </c>
+      <c r="G1508">
+        <v>70</v>
+      </c>
+      <c r="I1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1508" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1508">
+        <v>5</v>
+      </c>
+      <c r="X1508">
+        <v>5</v>
+      </c>
+      <c r="AF1508">
+        <v>10</v>
+      </c>
+      <c r="AU1508">
+        <v>3</v>
+      </c>
+      <c r="AV1508">
+        <v>2</v>
+      </c>
+      <c r="AY1508">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:87" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1509">
+        <v>2024</v>
+      </c>
+      <c r="B1509">
+        <v>11</v>
+      </c>
+      <c r="C1509">
+        <v>15</v>
+      </c>
+      <c r="D1509" s="3">
+        <v>0.47569444444444398</v>
+      </c>
+      <c r="E1509">
+        <v>0.3</v>
+      </c>
+      <c r="F1509">
+        <v>4</v>
+      </c>
+      <c r="G1509">
+        <v>75</v>
+      </c>
+      <c r="I1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="J1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="K1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="M1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="N1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="O1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="P1509" t="s">
+        <v>127</v>
+      </c>
+      <c r="R1509">
+        <v>10</v>
+      </c>
+      <c r="W1509">
+        <v>1</v>
+      </c>
+      <c r="X1509">
+        <v>2</v>
+      </c>
+      <c r="AF1509">
+        <v>50</v>
+      </c>
+      <c r="AU1509">
+        <v>5</v>
+      </c>
+      <c r="AV1509">
+        <v>5</v>
+      </c>
+      <c r="BA1509">
+        <v>1</v>
+      </c>
+      <c r="BD1509">
+        <v>1</v>
+      </c>
+      <c r="BE1509">
+        <v>2</v>
+      </c>
+      <c r="CE1509">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -60467,6 +63165,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="9ec2d0b7-503f-4434-bd5e-691963e6366e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C107646D0035FA4C8F1F95DBA74C7670" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1757c077ac40972b876cd5ccdf595ef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9ec2d0b7-503f-4434-bd5e-691963e6366e" xmlns:ns4="a169fe49-86d9-4b9f-a163-9271c3e82536" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="315eec8d60efed50e87e3fc3108bb7d6" ns3:_="" ns4:_="">
     <xsd:import namespace="9ec2d0b7-503f-4434-bd5e-691963e6366e"/>
@@ -60719,24 +63434,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E07FED4-9CAB-4D35-B6E3-4F76C1ACDD32}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9ec2d0b7-503f-4434-bd5e-691963e6366e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="9ec2d0b7-503f-4434-bd5e-691963e6366e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5801A-55FB-4B4B-B6DE-27DF63074F19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFBE69FB-5B7A-431F-9647-BD3868909ADD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -60753,22 +63469,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5801A-55FB-4B4B-B6DE-27DF63074F19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E07FED4-9CAB-4D35-B6E3-4F76C1ACDD32}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9ec2d0b7-503f-4434-bd5e-691963e6366e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
july 2025 and other updates
</commit_message>
<xml_diff>
--- a/GW_seaweed_seasonality_transect_data.xlsx
+++ b/GW_seaweed_seasonality_transect_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ubcca-my.sharepoint.com/personal/sschenk_student_ubc_ca/Documents/Project - Seaweed Seasonality Transects/seaweed_seasonality_2021-09-05/git_GW_seaweed_seasonality_transects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="771" documentId="13_ncr:1_{C3EE9921-92A6-4D79-9E53-9575D7FEA779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FBC5963-2C86-4F2C-A302-CCC1CEA48D20}"/>
+  <xr:revisionPtr revIDLastSave="774" documentId="13_ncr:1_{C3EE9921-92A6-4D79-9E53-9575D7FEA779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABBCC747-D502-43C5-A84A-FB0D0C3E1F50}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1359,9 +1359,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CY1819"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AZ1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1783" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AZ1820" sqref="AZ1820"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1782" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N1803" sqref="N1803"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1373,15 +1373,15 @@
     <col min="5" max="5" width="17.21875" customWidth="1"/>
     <col min="6" max="6" width="15.109375" customWidth="1"/>
     <col min="7" max="7" width="5.5546875" customWidth="1"/>
-    <col min="8" max="8" width="4.6640625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="7.109375" style="9" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="8.44140625" style="9" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="9" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="7.77734375" style="9" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" style="9" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="7.21875" style="9" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" style="9" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="7.44140625" style="9" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="4.6640625" customWidth="1"/>
+    <col min="9" max="9" width="7.109375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="8.44140625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="10" style="9" customWidth="1"/>
+    <col min="12" max="12" width="7.77734375" style="9" customWidth="1"/>
+    <col min="13" max="13" width="7.44140625" style="9" customWidth="1"/>
+    <col min="14" max="14" width="7.21875" style="9" customWidth="1"/>
+    <col min="15" max="15" width="6.33203125" style="9" customWidth="1"/>
+    <col min="16" max="16" width="7.44140625" style="9" customWidth="1"/>
     <col min="17" max="17" width="6.6640625" customWidth="1"/>
     <col min="18" max="18" width="7" customWidth="1"/>
     <col min="19" max="19" width="6.5546875" customWidth="1"/>
@@ -77907,15 +77907,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C107646D0035FA4C8F1F95DBA74C7670" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1757c077ac40972b876cd5ccdf595ef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9ec2d0b7-503f-4434-bd5e-691963e6366e" xmlns:ns4="a169fe49-86d9-4b9f-a163-9271c3e82536" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="315eec8d60efed50e87e3fc3108bb7d6" ns3:_="" ns4:_="">
     <xsd:import namespace="9ec2d0b7-503f-4434-bd5e-691963e6366e"/>
@@ -78168,6 +78159,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -78177,14 +78177,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5801A-55FB-4B4B-B6DE-27DF63074F19}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DFBE69FB-5B7A-431F-9647-BD3868909ADD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -78203,6 +78195,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{01C5801A-55FB-4B4B-B6DE-27DF63074F19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E07FED4-9CAB-4D35-B6E3-4F76C1ACDD32}">
   <ds:schemaRefs>

</xml_diff>